<commit_message>
Updating image outputs for the report
</commit_message>
<xml_diff>
--- a/charts_and_tables/tables/formatted_xls_tables/tbl_2021_summ_incis_by_type.xlsx
+++ b/charts_and_tables/tables/formatted_xls_tables/tbl_2021_summ_incis_by_type.xlsx
@@ -516,7 +516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -635,66 +635,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -865,6 +805,86 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -930,121 +950,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1093,7 +1113,38 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1372,7 +1423,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:R2"/>
+      <selection activeCell="I3" sqref="I3:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1396,1884 +1447,1884 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="34" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="34" t="s">
+      <c r="F1" s="36"/>
+      <c r="G1" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="34" t="s">
+      <c r="H1" s="36"/>
+      <c r="I1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="35"/>
-      <c r="K1" s="34" t="s">
+      <c r="J1" s="36"/>
+      <c r="K1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="38" t="s">
+      <c r="L1" s="36"/>
+      <c r="M1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="40"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="43"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="41" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="M2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="43" t="s">
+      <c r="N2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="O2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="43" t="s">
+      <c r="P2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="43" t="s">
+      <c r="Q2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="13">
         <v>31</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="14">
         <v>0.20512820512820501</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="17">
         <v>78</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="18">
         <v>-2.6315789473684199E-2</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="19">
         <v>7.5875486381323007E-2</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="18">
         <v>4.8561335244726701E-2</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="22">
         <v>2.1845068055788901</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="18">
         <v>-0.172016644703677</v>
       </c>
-      <c r="K3" s="31">
+      <c r="K3" s="25">
         <v>0.51428571428571401</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L3" s="18">
         <v>3.4101382488479298E-2</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="5">
         <v>2.5161290322580601</v>
       </c>
-      <c r="N3" s="10">
-        <v>1</v>
-      </c>
-      <c r="O3" s="10">
-        <v>1</v>
-      </c>
-      <c r="P3" s="10">
+      <c r="N3" s="6">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
         <v>20</v>
       </c>
-      <c r="Q3" s="10">
-        <v>1</v>
-      </c>
-      <c r="R3" s="11">
+      <c r="Q3" s="6">
+        <v>1</v>
+      </c>
+      <c r="R3" s="7">
         <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="33"/>
+      <c r="B4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="13">
         <v>0</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="14">
         <v>-1</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="13">
         <v>0</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="14">
         <v>-1</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="20">
         <v>0</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="14">
         <v>-1</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="13">
         <v>0</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="14">
         <v>-1</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="26">
         <v>0</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="14">
         <v>-0.09</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="5">
         <v>0</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="6">
         <v>0</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="6">
         <v>0</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="6">
         <v>0</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="6">
         <v>0</v>
       </c>
-      <c r="R4" s="11">
+      <c r="R4" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="13">
         <v>18</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="14">
         <v>-0.5</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="13">
         <v>55</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="14">
         <v>-1.5</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="20">
         <v>5.3501945525291798E-2</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="14">
         <v>-1.3176070038910499</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="23">
         <v>1.5403573629081899</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="14">
         <v>-1.8549123396628</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="26">
         <v>0.28571428571428598</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="14">
         <v>4.6082949308756099E-3</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="5">
         <v>3.0555555555555598</v>
       </c>
-      <c r="N5" s="10">
-        <v>1</v>
-      </c>
-      <c r="O5" s="10">
-        <v>1</v>
-      </c>
-      <c r="P5" s="10">
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6">
         <v>30</v>
       </c>
-      <c r="Q5" s="10">
-        <v>1</v>
-      </c>
-      <c r="R5" s="11">
+      <c r="Q5" s="6">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="33"/>
+      <c r="B6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="13">
         <v>36</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="14">
         <v>0.2</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="13">
         <v>87</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="14">
         <v>0.51396648044692705</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="20">
         <v>8.4630350194552506E-2</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="14">
         <v>0.54942612438319205</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="23">
         <v>2.4365652831456899</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="14">
         <v>0.44496676301527699</v>
       </c>
-      <c r="K6" s="32">
+      <c r="K6" s="26">
         <v>0.6</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="14">
         <v>-5.16129032258065E-2</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="5">
         <v>2.3888888888888902</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="6">
         <v>2</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="6">
         <v>0</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P6" s="6">
         <v>10</v>
       </c>
-      <c r="Q6" s="10">
-        <v>1</v>
-      </c>
-      <c r="R6" s="11">
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="13">
         <v>20</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="14">
         <v>0.28571428571428598</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="13">
         <v>101</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="14">
         <v>6.4814814814814797E-2</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="20">
         <v>9.8249027237354097E-2</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="14">
         <v>0.133043305951866</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="23">
         <v>2.8286562482495898</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="14">
         <v>-6.7948690022010996E-2</v>
       </c>
-      <c r="K7" s="32">
+      <c r="K7" s="26">
         <v>0.54285714285714304</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="14">
         <v>-9.1244239631336405E-2</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="5">
         <v>5</v>
       </c>
-      <c r="N7" s="10">
-        <v>1</v>
-      </c>
-      <c r="O7" s="10">
+      <c r="N7" s="6">
+        <v>1</v>
+      </c>
+      <c r="O7" s="6">
         <v>0</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="6">
         <v>58</v>
       </c>
-      <c r="Q7" s="10">
-        <v>1</v>
-      </c>
-      <c r="R7" s="11">
+      <c r="Q7" s="6">
+        <v>1</v>
+      </c>
+      <c r="R7" s="7">
         <v>3.25</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="13">
         <v>63</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="14">
         <v>-0.43181818181818199</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="13">
         <v>256</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="14">
         <v>3.03030303030303E-2</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="20">
         <v>0.249027237354086</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="14">
         <v>0.10104940455135</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="23">
         <v>7.1696633618999597</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="14">
         <v>-0.10735993780860199</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="26">
         <v>0.6</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="14">
         <v>-1.9354838709677399E-2</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="5">
         <v>4.0476190476190501</v>
       </c>
-      <c r="N8" s="10">
-        <v>1</v>
-      </c>
-      <c r="O8" s="10">
+      <c r="N8" s="6">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6">
         <v>0</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="6">
         <v>60</v>
       </c>
-      <c r="Q8" s="10">
-        <v>1</v>
-      </c>
-      <c r="R8" s="11">
+      <c r="Q8" s="6">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="13">
         <v>37</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="14">
         <v>5.1282051282051301E-2</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="13">
         <v>107</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="14">
         <v>-0.52857142857142903</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="20">
         <v>0.10408560311284</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="14">
         <v>-0.41705113952195699</v>
       </c>
-      <c r="I9" s="29">
+      <c r="I9" s="23">
         <v>2.9966952332941199</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="14">
         <v>-0.74557497339382806</v>
       </c>
-      <c r="K9" s="32">
+      <c r="K9" s="26">
         <v>0.57142857142857095</v>
       </c>
-      <c r="L9" s="20">
+      <c r="L9" s="14">
         <v>-8.7557603686635899E-2</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="5">
         <v>2.8918918918918899</v>
       </c>
-      <c r="N9" s="10">
-        <v>1</v>
-      </c>
-      <c r="O9" s="10">
-        <v>1</v>
-      </c>
-      <c r="P9" s="10">
+      <c r="N9" s="6">
+        <v>1</v>
+      </c>
+      <c r="O9" s="6">
+        <v>1</v>
+      </c>
+      <c r="P9" s="6">
         <v>39</v>
       </c>
-      <c r="Q9" s="10">
-        <v>1</v>
-      </c>
-      <c r="R9" s="11">
+      <c r="Q9" s="6">
+        <v>1</v>
+      </c>
+      <c r="R9" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="13">
         <v>7</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="14">
         <v>-1.3333333333333299</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="13">
         <v>7</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="14">
         <v>-1.3333333333333299</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="20">
         <v>6.80933852140078E-3</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="14">
         <v>-1.16309987029831</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="23">
         <v>0.19604548255195201</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="14">
         <v>-1.66458485035195</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="26">
         <v>0.14285714285714299</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="14">
         <v>-4.6082949308755797E-2</v>
       </c>
-      <c r="M10" s="9">
-        <v>1</v>
-      </c>
-      <c r="N10" s="10">
-        <v>1</v>
-      </c>
-      <c r="O10" s="10">
-        <v>1</v>
-      </c>
-      <c r="P10" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="10">
-        <v>1</v>
-      </c>
-      <c r="R10" s="11">
+      <c r="M10" s="5">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
+        <v>1</v>
+      </c>
+      <c r="P10" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>1</v>
+      </c>
+      <c r="R10" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="13">
         <v>37</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="14">
         <v>0.52564102564102599</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="13">
         <v>61</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="14">
         <v>0.67204301075268802</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="20">
         <v>5.9338521400778201E-2</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="14">
         <v>0.69596983389816303</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="23">
         <v>1.70839634795273</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="14">
         <v>0.62548461780767595</v>
       </c>
-      <c r="K11" s="32">
+      <c r="K11" s="26">
         <v>0.34285714285714303</v>
       </c>
-      <c r="L11" s="20">
+      <c r="L11" s="14">
         <v>0.23778801843318001</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="5">
         <v>1.64864864864865</v>
       </c>
-      <c r="N11" s="10">
-        <v>1</v>
-      </c>
-      <c r="O11" s="10">
-        <v>1</v>
-      </c>
-      <c r="P11" s="10">
+      <c r="N11" s="6">
+        <v>1</v>
+      </c>
+      <c r="O11" s="6">
+        <v>1</v>
+      </c>
+      <c r="P11" s="6">
         <v>5</v>
       </c>
-      <c r="Q11" s="10">
-        <v>1</v>
-      </c>
-      <c r="R11" s="11">
+      <c r="Q11" s="6">
+        <v>1</v>
+      </c>
+      <c r="R11" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="13">
         <v>125</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="14">
         <v>6.7164179104477598E-2</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="13">
         <v>208</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="14">
         <v>-9.7087378640776708E-3</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="20">
         <v>0.202334630350195</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="14">
         <v>6.3956782894488307E-2</v>
       </c>
-      <c r="I12" s="29">
+      <c r="I12" s="23">
         <v>5.82535148154372</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="14">
         <v>-0.15305197407740301</v>
       </c>
-      <c r="K12" s="32">
+      <c r="K12" s="26">
         <v>0.68571428571428605</v>
       </c>
-      <c r="L12" s="20">
+      <c r="L12" s="14">
         <v>0.12073732718893999</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="5">
         <v>1.6639999999999999</v>
       </c>
-      <c r="N12" s="10">
-        <v>1</v>
-      </c>
-      <c r="O12" s="10">
-        <v>1</v>
-      </c>
-      <c r="P12" s="10">
+      <c r="N12" s="6">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1</v>
+      </c>
+      <c r="P12" s="6">
         <v>6</v>
       </c>
-      <c r="Q12" s="10">
-        <v>1</v>
-      </c>
-      <c r="R12" s="11">
+      <c r="Q12" s="6">
+        <v>1</v>
+      </c>
+      <c r="R12" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="13">
         <v>23</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="14">
         <v>-0.53333333333333299</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="13">
         <v>50</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="14">
         <v>0.34210526315789502</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="20">
         <v>4.8638132295719803E-2</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="14">
         <v>0.39010342002867099</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="23">
         <v>1.40032487537109</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="14">
         <v>0.24870727903610501</v>
       </c>
-      <c r="K13" s="32">
+      <c r="K13" s="26">
         <v>0.25714285714285701</v>
       </c>
-      <c r="L13" s="20">
+      <c r="L13" s="14">
         <v>-0.12811059907834099</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="5">
         <v>2.1739130434782599</v>
       </c>
-      <c r="N13" s="10">
-        <v>1</v>
-      </c>
-      <c r="O13" s="10">
-        <v>1</v>
-      </c>
-      <c r="P13" s="10">
+      <c r="N13" s="6">
+        <v>1</v>
+      </c>
+      <c r="O13" s="6">
+        <v>1</v>
+      </c>
+      <c r="P13" s="6">
         <v>10</v>
       </c>
-      <c r="Q13" s="10">
-        <v>1</v>
-      </c>
-      <c r="R13" s="11">
+      <c r="Q13" s="6">
+        <v>1</v>
+      </c>
+      <c r="R13" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="33"/>
+      <c r="B14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="13">
         <v>53</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="14">
         <v>-0.15217391304347799</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="13">
         <v>219</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="14">
         <v>-1.8604651162790701E-2</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="20">
         <v>0.21303501945525299</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="14">
         <v>5.5709890507646298E-2</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="23">
         <v>6.1334229541253604</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="14">
         <v>-0.16321079513702999</v>
       </c>
-      <c r="K14" s="32">
+      <c r="K14" s="26">
         <v>0.2</v>
       </c>
-      <c r="L14" s="20">
+      <c r="L14" s="14">
         <v>-6.4516129032258203E-3</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="5">
         <v>4.1320754716981103</v>
       </c>
-      <c r="N14" s="10">
-        <v>1</v>
-      </c>
-      <c r="O14" s="10">
-        <v>1</v>
-      </c>
-      <c r="P14" s="10">
+      <c r="N14" s="6">
+        <v>1</v>
+      </c>
+      <c r="O14" s="6">
+        <v>1</v>
+      </c>
+      <c r="P14" s="6">
         <v>60</v>
       </c>
-      <c r="Q14" s="10">
-        <v>1</v>
-      </c>
-      <c r="R14" s="11">
+      <c r="Q14" s="6">
+        <v>1</v>
+      </c>
+      <c r="R14" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="13">
         <v>2</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="14">
         <v>0.81818181818181801</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="13">
         <v>25</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="14">
         <v>0.73958333333333304</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="20">
         <v>2.4319066147859902E-2</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="14">
         <v>0.75858260376134901</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="23">
         <v>0.70016243768554298</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="14">
         <v>0.70261329795179195</v>
       </c>
-      <c r="K15" s="32">
+      <c r="K15" s="26">
         <v>5.7142857142857099E-2</v>
       </c>
-      <c r="L15" s="20">
+      <c r="L15" s="14">
         <v>7.3732718894009199E-3</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="5">
         <v>12.5</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="6">
         <v>12.5</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="6">
         <v>2</v>
       </c>
-      <c r="P15" s="10">
+      <c r="P15" s="6">
         <v>23</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="6">
         <v>7.25</v>
       </c>
-      <c r="R15" s="11">
+      <c r="R15" s="7">
         <v>17.75</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="33"/>
+      <c r="B16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="13">
         <v>24</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="14">
         <v>-2.4285714285714302</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="13">
         <v>160</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="14">
         <v>-1.6229508196721301</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="20">
         <v>0.155642023346304</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="14">
         <v>-1.43158767621356</v>
       </c>
-      <c r="I16" s="29">
+      <c r="I16" s="23">
         <v>4.4810396011874802</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="14">
         <v>-1.99531786456425</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16" s="26">
         <v>0.14285714285714299</v>
       </c>
-      <c r="L16" s="20">
+      <c r="L16" s="14">
         <v>5.0691244239631297E-2</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="5">
         <v>6.6666666666666696</v>
       </c>
-      <c r="N16" s="10">
-        <v>1</v>
-      </c>
-      <c r="O16" s="10">
-        <v>1</v>
-      </c>
-      <c r="P16" s="10">
+      <c r="N16" s="6">
+        <v>1</v>
+      </c>
+      <c r="O16" s="6">
+        <v>1</v>
+      </c>
+      <c r="P16" s="6">
         <v>48</v>
       </c>
-      <c r="Q16" s="10">
-        <v>1</v>
-      </c>
-      <c r="R16" s="11">
+      <c r="Q16" s="6">
+        <v>1</v>
+      </c>
+      <c r="R16" s="7">
         <v>5.25</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="33"/>
+      <c r="B17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="19">
-        <v>1</v>
-      </c>
-      <c r="D17" s="20">
-        <v>1</v>
-      </c>
-      <c r="E17" s="19">
-        <v>1</v>
-      </c>
-      <c r="F17" s="20">
-        <v>1</v>
-      </c>
-      <c r="G17" s="26">
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
+        <v>1</v>
+      </c>
+      <c r="F17" s="14">
+        <v>1</v>
+      </c>
+      <c r="G17" s="20">
         <v>9.7276264591439701E-4</v>
       </c>
-      <c r="H17" s="20">
-        <v>1</v>
-      </c>
-      <c r="I17" s="29">
+      <c r="H17" s="14">
+        <v>1</v>
+      </c>
+      <c r="I17" s="23">
         <v>2.80064975074217E-2</v>
       </c>
-      <c r="J17" s="20">
-        <v>1</v>
-      </c>
-      <c r="K17" s="32">
+      <c r="J17" s="14">
+        <v>1</v>
+      </c>
+      <c r="K17" s="26">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="L17" s="20">
+      <c r="L17" s="14">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="M17" s="9">
-        <v>1</v>
-      </c>
-      <c r="N17" s="10">
-        <v>1</v>
-      </c>
-      <c r="O17" s="10">
-        <v>1</v>
-      </c>
-      <c r="P17" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="10">
-        <v>1</v>
-      </c>
-      <c r="R17" s="11">
+      <c r="M17" s="5">
+        <v>1</v>
+      </c>
+      <c r="N17" s="6">
+        <v>1</v>
+      </c>
+      <c r="O17" s="6">
+        <v>1</v>
+      </c>
+      <c r="P17" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>1</v>
+      </c>
+      <c r="R17" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="13">
         <v>34</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="14">
         <v>0.29166666666666702</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="13">
         <v>191</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="14">
         <v>-0.38405797101449302</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="20">
         <v>0.18579766536965001</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="14">
         <v>-0.28308097896577</v>
       </c>
-      <c r="I18" s="29">
+      <c r="I18" s="23">
         <v>5.3492410239175499</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="14">
         <v>-0.58054567210317398</v>
       </c>
-      <c r="K18" s="32">
+      <c r="K18" s="26">
         <v>0.2</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L18" s="14">
         <v>-6.4516129032258203E-3</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="5">
         <v>5.6176470588235299</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="6">
         <v>2</v>
       </c>
-      <c r="O18" s="10">
-        <v>1</v>
-      </c>
-      <c r="P18" s="10">
+      <c r="O18" s="6">
+        <v>1</v>
+      </c>
+      <c r="P18" s="6">
         <v>100</v>
       </c>
-      <c r="Q18" s="10">
-        <v>1</v>
-      </c>
-      <c r="R18" s="11">
+      <c r="Q18" s="6">
+        <v>1</v>
+      </c>
+      <c r="R18" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="33"/>
+      <c r="B19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="13">
         <v>22</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="14">
         <v>-4.7619047619047603E-2</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="13">
         <v>137</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="14">
         <v>0.179640718562874</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="20">
         <v>0.13326848249027201</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="14">
         <v>0.239491833453715</v>
       </c>
-      <c r="I19" s="29">
+      <c r="I19" s="23">
         <v>3.8368901585167801</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="14">
         <v>6.3178465787296301E-2</v>
       </c>
-      <c r="K19" s="32">
+      <c r="K19" s="26">
         <v>0.14285714285714299</v>
       </c>
-      <c r="L19" s="20">
+      <c r="L19" s="14">
         <v>1.8433179723502301E-2</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="5">
         <v>6.2272727272727302</v>
       </c>
-      <c r="N19" s="10">
-        <v>1</v>
-      </c>
-      <c r="O19" s="10">
-        <v>1</v>
-      </c>
-      <c r="P19" s="10">
+      <c r="N19" s="6">
+        <v>1</v>
+      </c>
+      <c r="O19" s="6">
+        <v>1</v>
+      </c>
+      <c r="P19" s="6">
         <v>50</v>
       </c>
-      <c r="Q19" s="10">
-        <v>1</v>
-      </c>
-      <c r="R19" s="11">
+      <c r="Q19" s="6">
+        <v>1</v>
+      </c>
+      <c r="R19" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="33"/>
+      <c r="B20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="13">
         <v>15</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="14">
         <v>0.16666666666666699</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="13">
         <v>58</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="14">
         <v>-0.28888888888888897</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="20">
         <v>5.6420233463034999E-2</v>
       </c>
-      <c r="H20" s="20">
+      <c r="H20" s="14">
         <v>-0.194855166450497</v>
       </c>
-      <c r="I20" s="29">
+      <c r="I20" s="23">
         <v>1.6243768554304601</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="14">
         <v>-0.47186591733726702</v>
       </c>
-      <c r="K20" s="32">
+      <c r="K20" s="26">
         <v>0.14285714285714299</v>
       </c>
-      <c r="L20" s="20">
+      <c r="L20" s="14">
         <v>5.0691244239631297E-2</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="5">
         <v>3.8666666666666698</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="6">
         <v>2</v>
       </c>
-      <c r="O20" s="10">
-        <v>1</v>
-      </c>
-      <c r="P20" s="10">
+      <c r="O20" s="6">
+        <v>1</v>
+      </c>
+      <c r="P20" s="6">
         <v>15</v>
       </c>
-      <c r="Q20" s="10">
-        <v>1</v>
-      </c>
-      <c r="R20" s="11">
+      <c r="Q20" s="6">
+        <v>1</v>
+      </c>
+      <c r="R20" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16" t="s">
+      <c r="A21" s="33"/>
+      <c r="B21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="13">
         <v>20</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="14">
         <v>-5.2631578947368397E-2</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="13">
         <v>691</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="14">
         <v>-1.4416961130742001</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="20">
         <v>0.67217898832684797</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="14">
         <v>-1.26355680521373</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="23">
         <v>19.352489777628399</v>
       </c>
-      <c r="J21" s="20">
+      <c r="J21" s="14">
         <v>-1.7883313451689</v>
       </c>
-      <c r="K21" s="32">
+      <c r="K21" s="26">
         <v>0.25714285714285701</v>
       </c>
-      <c r="L21" s="20">
+      <c r="L21" s="14">
         <v>-3.1336405529953898E-2</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="5">
         <v>34.549999999999997</v>
       </c>
-      <c r="N21" s="10">
+      <c r="N21" s="6">
         <v>18</v>
       </c>
-      <c r="O21" s="10">
-        <v>1</v>
-      </c>
-      <c r="P21" s="10">
+      <c r="O21" s="6">
+        <v>1</v>
+      </c>
+      <c r="P21" s="6">
         <v>400</v>
       </c>
-      <c r="Q21" s="10">
-        <v>1</v>
-      </c>
-      <c r="R21" s="11">
+      <c r="Q21" s="6">
+        <v>1</v>
+      </c>
+      <c r="R21" s="7">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16" t="s">
+      <c r="A22" s="33"/>
+      <c r="B22" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="13">
         <v>3</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="14">
         <v>-0.5</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="13">
         <v>5</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="14">
         <v>-0.66666666666666696</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="20">
         <v>4.8638132295719802E-3</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="14">
         <v>-0.54507133592736701</v>
       </c>
-      <c r="I22" s="29">
+      <c r="I22" s="23">
         <v>0.14003248753710901</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="14">
         <v>-0.90327489310853504</v>
       </c>
-      <c r="K22" s="32">
+      <c r="K22" s="26">
         <v>0.17142857142857101</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L22" s="14">
         <v>-0.10691244239631301</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="5">
         <v>1.6666666666666701</v>
       </c>
-      <c r="N22" s="10">
+      <c r="N22" s="6">
         <v>2</v>
       </c>
-      <c r="O22" s="10">
-        <v>1</v>
-      </c>
-      <c r="P22" s="10">
+      <c r="O22" s="6">
+        <v>1</v>
+      </c>
+      <c r="P22" s="6">
         <v>2</v>
       </c>
-      <c r="Q22" s="10">
+      <c r="Q22" s="6">
         <v>1.5</v>
       </c>
-      <c r="R22" s="11">
+      <c r="R22" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="13">
         <v>27</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="14">
         <v>0.27027027027027001</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="13">
         <v>147</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="14">
         <v>1.34228187919463E-2</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="20">
         <v>0.142996108949416</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="14">
         <v>8.5400725981249898E-2</v>
       </c>
-      <c r="I23" s="29">
+      <c r="I23" s="23">
         <v>4.1169551335909897</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J23" s="14">
         <v>-0.12663654746424599</v>
       </c>
-      <c r="K23" s="32">
+      <c r="K23" s="26">
         <v>0.57142857142857095</v>
       </c>
-      <c r="L23" s="20">
+      <c r="L23" s="14">
         <v>-5.5299539170506902E-2</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="5">
         <v>5.4444444444444402</v>
       </c>
-      <c r="N23" s="10">
-        <v>1</v>
-      </c>
-      <c r="O23" s="10">
-        <v>1</v>
-      </c>
-      <c r="P23" s="10">
+      <c r="N23" s="6">
+        <v>1</v>
+      </c>
+      <c r="O23" s="6">
+        <v>1</v>
+      </c>
+      <c r="P23" s="6">
         <v>50</v>
       </c>
-      <c r="Q23" s="10">
-        <v>1</v>
-      </c>
-      <c r="R23" s="11">
+      <c r="Q23" s="6">
+        <v>1</v>
+      </c>
+      <c r="R23" s="7">
         <v>3.5</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16" t="s">
+      <c r="A24" s="33"/>
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="13">
         <v>3</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="14">
         <v>0.4</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="13">
         <v>14</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="14">
         <v>0.875</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="20">
         <v>1.36186770428016E-2</v>
       </c>
-      <c r="H24" s="20">
+      <c r="H24" s="14">
         <v>0.88411964980544699</v>
       </c>
-      <c r="I24" s="29">
+      <c r="I24" s="23">
         <v>0.39209096510390401</v>
       </c>
-      <c r="J24" s="20">
+      <c r="J24" s="14">
         <v>0.85725438301685997</v>
       </c>
-      <c r="K24" s="32">
+      <c r="K24" s="26">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="L24" s="20">
+      <c r="L24" s="14">
         <v>1.10599078341014E-2</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M24" s="5">
         <v>4.6666666666666696</v>
       </c>
-      <c r="N24" s="10">
-        <v>1</v>
-      </c>
-      <c r="O24" s="10">
-        <v>1</v>
-      </c>
-      <c r="P24" s="10">
+      <c r="N24" s="6">
+        <v>1</v>
+      </c>
+      <c r="O24" s="6">
+        <v>1</v>
+      </c>
+      <c r="P24" s="6">
         <v>12</v>
       </c>
-      <c r="Q24" s="10">
-        <v>1</v>
-      </c>
-      <c r="R24" s="11">
+      <c r="Q24" s="6">
+        <v>1</v>
+      </c>
+      <c r="R24" s="7">
         <v>6.5</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16" t="s">
+      <c r="A25" s="33"/>
+      <c r="B25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="19">
-        <v>1</v>
-      </c>
-      <c r="D25" s="20">
-        <v>1</v>
-      </c>
-      <c r="E25" s="19">
-        <v>1</v>
-      </c>
-      <c r="F25" s="20">
-        <v>1</v>
-      </c>
-      <c r="G25" s="26">
+      <c r="C25" s="13">
+        <v>1</v>
+      </c>
+      <c r="D25" s="14">
+        <v>1</v>
+      </c>
+      <c r="E25" s="13">
+        <v>1</v>
+      </c>
+      <c r="F25" s="14">
+        <v>1</v>
+      </c>
+      <c r="G25" s="20">
         <v>9.7276264591439701E-4</v>
       </c>
-      <c r="H25" s="20">
-        <v>1</v>
-      </c>
-      <c r="I25" s="29">
+      <c r="H25" s="14">
+        <v>1</v>
+      </c>
+      <c r="I25" s="23">
         <v>2.80064975074217E-2</v>
       </c>
-      <c r="J25" s="20">
-        <v>1</v>
-      </c>
-      <c r="K25" s="32">
+      <c r="J25" s="14">
+        <v>1</v>
+      </c>
+      <c r="K25" s="26">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="L25" s="20">
+      <c r="L25" s="14">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="M25" s="9">
-        <v>1</v>
-      </c>
-      <c r="N25" s="10">
-        <v>1</v>
-      </c>
-      <c r="O25" s="10">
-        <v>1</v>
-      </c>
-      <c r="P25" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="10">
-        <v>1</v>
-      </c>
-      <c r="R25" s="11">
+      <c r="M25" s="5">
+        <v>1</v>
+      </c>
+      <c r="N25" s="6">
+        <v>1</v>
+      </c>
+      <c r="O25" s="6">
+        <v>1</v>
+      </c>
+      <c r="P25" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>1</v>
+      </c>
+      <c r="R25" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16" t="s">
+      <c r="A26" s="33"/>
+      <c r="B26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="13">
         <v>2</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="14">
         <v>-1</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="13">
         <v>30</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="14">
         <v>-1</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="20">
         <v>2.91828793774319E-2</v>
       </c>
-      <c r="H26" s="20">
+      <c r="H26" s="14">
         <v>-0.85408560311284099</v>
       </c>
-      <c r="I26" s="29">
+      <c r="I26" s="23">
         <v>0.84019492522265204</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="14">
         <v>-1.2839298717302401</v>
       </c>
-      <c r="K26" s="32">
+      <c r="K26" s="26">
         <v>5.7142857142857099E-2</v>
       </c>
-      <c r="L26" s="20">
+      <c r="L26" s="14">
         <v>-2.4884792626728099E-2</v>
       </c>
-      <c r="M26" s="9">
+      <c r="M26" s="5">
         <v>15</v>
       </c>
-      <c r="N26" s="10">
+      <c r="N26" s="6">
         <v>15</v>
       </c>
-      <c r="O26" s="10">
+      <c r="O26" s="6">
         <v>10</v>
       </c>
-      <c r="P26" s="10">
+      <c r="P26" s="6">
         <v>20</v>
       </c>
-      <c r="Q26" s="10">
+      <c r="Q26" s="6">
         <v>12.5</v>
       </c>
-      <c r="R26" s="11">
+      <c r="R26" s="7">
         <v>17.5</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16" t="s">
+      <c r="A27" s="33"/>
+      <c r="B27" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="13">
         <v>3</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="14">
         <v>-0.5</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="13">
         <v>4</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="14">
         <v>-0.33333333333333298</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="20">
         <v>3.8910505836575902E-3</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="14">
         <v>-0.236057068741894</v>
       </c>
-      <c r="I27" s="29">
+      <c r="I27" s="23">
         <v>0.11202599002968699</v>
       </c>
-      <c r="J27" s="20">
+      <c r="J27" s="14">
         <v>-0.52261991448682799</v>
       </c>
-      <c r="K27" s="32">
+      <c r="K27" s="26">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="L27" s="20">
+      <c r="L27" s="14">
         <v>-5.3456221198156698E-2</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="5">
         <v>1.3333333333333299</v>
       </c>
-      <c r="N27" s="10">
-        <v>1</v>
-      </c>
-      <c r="O27" s="10">
-        <v>1</v>
-      </c>
-      <c r="P27" s="10">
+      <c r="N27" s="6">
+        <v>1</v>
+      </c>
+      <c r="O27" s="6">
+        <v>1</v>
+      </c>
+      <c r="P27" s="6">
         <v>2</v>
       </c>
-      <c r="Q27" s="10">
-        <v>1</v>
-      </c>
-      <c r="R27" s="11">
+      <c r="Q27" s="6">
+        <v>1</v>
+      </c>
+      <c r="R27" s="7">
         <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="19">
+      <c r="B28" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="13">
         <v>25</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="14">
         <v>-0.78571428571428603</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="13">
         <v>38</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="14">
         <v>-0.52</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="20">
         <v>3.6964980544747103E-2</v>
       </c>
-      <c r="H28" s="20">
+      <c r="H28" s="14">
         <v>-0.409105058365759</v>
       </c>
-      <c r="I28" s="29">
+      <c r="I28" s="23">
         <v>1.06424690528203</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J28" s="14">
         <v>-0.73578670251498302</v>
       </c>
-      <c r="K28" s="32">
+      <c r="K28" s="26">
         <v>0.45714285714285702</v>
       </c>
-      <c r="L28" s="20">
+      <c r="L28" s="14">
         <v>-0.13456221198156701</v>
       </c>
-      <c r="M28" s="9">
+      <c r="M28" s="5">
         <v>1.52</v>
       </c>
-      <c r="N28" s="10">
-        <v>1</v>
-      </c>
-      <c r="O28" s="10">
-        <v>1</v>
-      </c>
-      <c r="P28" s="10">
+      <c r="N28" s="6">
+        <v>1</v>
+      </c>
+      <c r="O28" s="6">
+        <v>1</v>
+      </c>
+      <c r="P28" s="6">
         <v>4</v>
       </c>
-      <c r="Q28" s="10">
-        <v>1</v>
-      </c>
-      <c r="R28" s="11">
+      <c r="Q28" s="6">
+        <v>1</v>
+      </c>
+      <c r="R28" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="13">
         <v>26</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="14">
         <v>0.31578947368421101</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="13">
         <v>309</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="14">
         <v>-0.21176470588235299</v>
       </c>
-      <c r="G29" s="26">
+      <c r="G29" s="20">
         <v>0.30058365758754901</v>
       </c>
-      <c r="H29" s="20">
+      <c r="H29" s="14">
         <v>-0.123357747768368</v>
       </c>
-      <c r="I29" s="29">
+      <c r="I29" s="23">
         <v>8.6540077297933102</v>
       </c>
-      <c r="J29" s="20">
+      <c r="J29" s="14">
         <v>-0.38379280463655802</v>
       </c>
-      <c r="K29" s="32">
+      <c r="K29" s="26">
         <v>0.28571428571428598</v>
       </c>
-      <c r="L29" s="20">
+      <c r="L29" s="14">
         <v>0.29493087557603698</v>
       </c>
-      <c r="M29" s="9">
+      <c r="M29" s="5">
         <v>11.884615384615399</v>
       </c>
-      <c r="N29" s="10">
+      <c r="N29" s="6">
         <v>2</v>
       </c>
-      <c r="O29" s="10">
-        <v>1</v>
-      </c>
-      <c r="P29" s="10">
+      <c r="O29" s="6">
+        <v>1</v>
+      </c>
+      <c r="P29" s="6">
         <v>100</v>
       </c>
-      <c r="Q29" s="10">
-        <v>1</v>
-      </c>
-      <c r="R29" s="11">
+      <c r="Q29" s="6">
+        <v>1</v>
+      </c>
+      <c r="R29" s="7">
         <v>7.5</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16" t="s">
+      <c r="A30" s="33"/>
+      <c r="B30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="13">
         <v>18</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="14">
         <v>-5.8823529411764698E-2</v>
       </c>
-      <c r="E30" s="19">
+      <c r="E30" s="13">
         <v>71</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="14">
         <v>-0.22413793103448301</v>
       </c>
-      <c r="G30" s="26">
+      <c r="G30" s="20">
         <v>6.9066147859922197E-2</v>
       </c>
-      <c r="H30" s="20">
+      <c r="H30" s="14">
         <v>-0.134828257077687</v>
       </c>
-      <c r="I30" s="29">
+      <c r="I30" s="23">
         <v>1.9884613230269399</v>
       </c>
-      <c r="J30" s="20">
+      <c r="J30" s="14">
         <v>-0.39792259390385498</v>
       </c>
-      <c r="K30" s="32">
+      <c r="K30" s="26">
         <v>0.314285714285714</v>
       </c>
-      <c r="L30" s="20">
+      <c r="L30" s="14">
         <v>-5.6221198156682001E-2</v>
       </c>
-      <c r="M30" s="9">
+      <c r="M30" s="5">
         <v>3.9444444444444402</v>
       </c>
-      <c r="N30" s="10">
-        <v>1</v>
-      </c>
-      <c r="O30" s="10">
-        <v>1</v>
-      </c>
-      <c r="P30" s="10">
+      <c r="N30" s="6">
+        <v>1</v>
+      </c>
+      <c r="O30" s="6">
+        <v>1</v>
+      </c>
+      <c r="P30" s="6">
         <v>40</v>
       </c>
-      <c r="Q30" s="10">
-        <v>1</v>
-      </c>
-      <c r="R30" s="11">
+      <c r="Q30" s="6">
+        <v>1</v>
+      </c>
+      <c r="R30" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="15"/>
-      <c r="B31" s="16" t="s">
+      <c r="A31" s="33"/>
+      <c r="B31" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="13">
         <v>8</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="14">
         <v>-0.6</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="13">
         <v>66</v>
       </c>
-      <c r="F31" s="20">
+      <c r="F31" s="14">
         <v>-2.8823529411764701</v>
       </c>
-      <c r="G31" s="26">
+      <c r="G31" s="20">
         <v>6.4202334630350202E-2</v>
       </c>
-      <c r="H31" s="20">
+      <c r="H31" s="14">
         <v>-2.5991073472190398</v>
       </c>
-      <c r="I31" s="29">
+      <c r="I31" s="23">
         <v>1.8484288354898299</v>
       </c>
-      <c r="J31" s="20">
+      <c r="J31" s="14">
         <v>-3.43351092747635</v>
       </c>
-      <c r="K31" s="32">
+      <c r="K31" s="26">
         <v>0.17142857142857101</v>
       </c>
-      <c r="L31" s="20">
+      <c r="L31" s="14">
         <v>8.6635944700460807E-2</v>
       </c>
-      <c r="M31" s="9">
+      <c r="M31" s="5">
         <v>8.25</v>
       </c>
-      <c r="N31" s="10">
+      <c r="N31" s="6">
         <v>7</v>
       </c>
-      <c r="O31" s="10">
-        <v>1</v>
-      </c>
-      <c r="P31" s="10">
+      <c r="O31" s="6">
+        <v>1</v>
+      </c>
+      <c r="P31" s="6">
         <v>23</v>
       </c>
-      <c r="Q31" s="10">
+      <c r="Q31" s="6">
         <v>1.75</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="7">
         <v>11.25</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16" t="s">
+      <c r="A32" s="33"/>
+      <c r="B32" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="13">
         <v>12</v>
       </c>
-      <c r="D32" s="20">
+      <c r="D32" s="14">
         <v>-0.33333333333333298</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="13">
         <v>30</v>
       </c>
-      <c r="F32" s="20">
+      <c r="F32" s="14">
         <v>-2.3333333333333299</v>
       </c>
-      <c r="G32" s="26">
+      <c r="G32" s="20">
         <v>2.91828793774319E-2</v>
       </c>
-      <c r="H32" s="20">
+      <c r="H32" s="14">
         <v>-2.0901426718547298</v>
       </c>
-      <c r="I32" s="29">
+      <c r="I32" s="23">
         <v>0.84019492522265204</v>
       </c>
-      <c r="J32" s="20">
+      <c r="J32" s="14">
         <v>-2.8065497862170701</v>
       </c>
-      <c r="K32" s="32">
+      <c r="K32" s="26">
         <v>0.25714285714285701</v>
       </c>
-      <c r="L32" s="20">
+      <c r="L32" s="14">
         <v>3.3179723502304199E-2</v>
       </c>
-      <c r="M32" s="9">
+      <c r="M32" s="5">
         <v>2.5</v>
       </c>
-      <c r="N32" s="10">
-        <v>1</v>
-      </c>
-      <c r="O32" s="10">
-        <v>1</v>
-      </c>
-      <c r="P32" s="10">
+      <c r="N32" s="6">
+        <v>1</v>
+      </c>
+      <c r="O32" s="6">
+        <v>1</v>
+      </c>
+      <c r="P32" s="6">
         <v>10</v>
       </c>
-      <c r="Q32" s="10">
-        <v>1</v>
-      </c>
-      <c r="R32" s="11">
+      <c r="Q32" s="6">
+        <v>1</v>
+      </c>
+      <c r="R32" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16" t="s">
+      <c r="A33" s="33"/>
+      <c r="B33" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="13">
         <v>25</v>
       </c>
-      <c r="D33" s="20">
+      <c r="D33" s="14">
         <v>7.4074074074074098E-2</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="13">
         <v>184</v>
       </c>
-      <c r="F33" s="20">
+      <c r="F33" s="14">
         <v>-5.7471264367816098E-2</v>
       </c>
-      <c r="G33" s="26">
+      <c r="G33" s="20">
         <v>0.178988326848249</v>
       </c>
-      <c r="H33" s="20">
+      <c r="H33" s="14">
         <v>1.9678876515049799E-2</v>
       </c>
-      <c r="I33" s="29">
+      <c r="I33" s="23">
         <v>5.1531955413655997</v>
       </c>
-      <c r="J33" s="20">
+      <c r="J33" s="14">
         <v>-0.20759510459300101</v>
       </c>
-      <c r="K33" s="32">
+      <c r="K33" s="26">
         <v>0.51428571428571401</v>
       </c>
-      <c r="L33" s="20">
+      <c r="L33" s="14">
         <v>3.4101382488479298E-2</v>
       </c>
-      <c r="M33" s="9">
+      <c r="M33" s="5">
         <v>7.36</v>
       </c>
-      <c r="N33" s="10">
-        <v>1</v>
-      </c>
-      <c r="O33" s="10">
-        <v>1</v>
-      </c>
-      <c r="P33" s="10">
+      <c r="N33" s="6">
+        <v>1</v>
+      </c>
+      <c r="O33" s="6">
+        <v>1</v>
+      </c>
+      <c r="P33" s="6">
         <v>70</v>
       </c>
-      <c r="Q33" s="10">
-        <v>1</v>
-      </c>
-      <c r="R33" s="11">
+      <c r="Q33" s="6">
+        <v>1</v>
+      </c>
+      <c r="R33" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="15"/>
-      <c r="B34" s="16" t="s">
+      <c r="A34" s="33"/>
+      <c r="B34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="13">
         <v>89</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="14">
         <v>2.1978021978022001E-2</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="13">
         <v>792</v>
       </c>
-      <c r="F34" s="20">
+      <c r="F34" s="14">
         <v>-2.9908972691807499E-2</v>
       </c>
-      <c r="G34" s="26">
+      <c r="G34" s="20">
         <v>0.77042801556420204</v>
       </c>
-      <c r="H34" s="20">
+      <c r="H34" s="14">
         <v>4.5230300607692002E-2</v>
       </c>
-      <c r="I34" s="29">
+      <c r="I34" s="23">
         <v>22.181146025878</v>
       </c>
-      <c r="J34" s="20">
+      <c r="J34" s="14">
         <v>-0.176119933946912</v>
       </c>
-      <c r="K34" s="32">
+      <c r="K34" s="26">
         <v>0.82857142857142896</v>
       </c>
-      <c r="L34" s="20">
+      <c r="L34" s="14">
         <v>-2.21198156682029E-2</v>
       </c>
-      <c r="M34" s="9">
+      <c r="M34" s="5">
         <v>8.8988764044943807</v>
       </c>
-      <c r="N34" s="10">
+      <c r="N34" s="6">
         <v>2</v>
       </c>
-      <c r="O34" s="10">
-        <v>1</v>
-      </c>
-      <c r="P34" s="10">
+      <c r="O34" s="6">
+        <v>1</v>
+      </c>
+      <c r="P34" s="6">
         <v>102</v>
       </c>
-      <c r="Q34" s="10">
-        <v>1</v>
-      </c>
-      <c r="R34" s="11">
+      <c r="Q34" s="6">
+        <v>1</v>
+      </c>
+      <c r="R34" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="17"/>
-      <c r="B35" s="18" t="s">
+      <c r="A35" s="34"/>
+      <c r="B35" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="15">
         <v>8</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="16">
         <v>-0.14285714285714299</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="15">
         <v>71</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="16">
         <v>0.15476190476190499</v>
       </c>
-      <c r="G35" s="27">
+      <c r="G35" s="21">
         <v>6.9066147859922197E-2</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="16">
         <v>0.216428108208264</v>
       </c>
-      <c r="I35" s="30">
+      <c r="I35" s="24">
         <v>1.9884613230269399</v>
       </c>
-      <c r="J35" s="22">
+      <c r="J35" s="16">
         <v>3.4767732780671898E-2</v>
       </c>
-      <c r="K35" s="33">
+      <c r="K35" s="27">
         <v>0.34285714285714303</v>
       </c>
-      <c r="L35" s="22">
+      <c r="L35" s="16">
         <v>-0.14930875576036901</v>
       </c>
-      <c r="M35" s="12">
+      <c r="M35" s="8">
         <v>8.875</v>
       </c>
-      <c r="N35" s="13">
+      <c r="N35" s="9">
         <v>4</v>
       </c>
-      <c r="O35" s="13">
-        <v>1</v>
-      </c>
-      <c r="P35" s="13">
+      <c r="O35" s="9">
+        <v>1</v>
+      </c>
+      <c r="P35" s="9">
         <v>30</v>
       </c>
-      <c r="Q35" s="13">
-        <v>1</v>
-      </c>
-      <c r="R35" s="14">
+      <c r="Q35" s="9">
+        <v>1</v>
+      </c>
+      <c r="R35" s="10">
         <v>12.5</v>
       </c>
     </row>
@@ -3295,7 +3346,7 @@
     <mergeCell ref="A9:A12"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D35">
-    <cfRule type="iconSet" priority="9">
+    <cfRule type="iconSet" priority="13">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="-0.3"/>
@@ -3306,6 +3357,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3 F5:F35">
+    <cfRule type="iconSet" priority="12">
+      <iconSet iconSet="5Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="-0.3"/>
+        <cfvo type="num" val="-1E-3"/>
+        <cfvo type="num" val="1E-3"/>
+        <cfvo type="num" val="0.3"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3 H5:H35">
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="5Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="-0.3"/>
+        <cfvo type="num" val="-1E-3"/>
+        <cfvo type="num" val="1E-3"/>
+        <cfvo type="num" val="0.3"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3 J5:J35">
+    <cfRule type="iconSet" priority="10">
+      <iconSet iconSet="5Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="-0.3"/>
+        <cfvo type="num" val="-1E-3"/>
+        <cfvo type="num" val="1E-3"/>
+        <cfvo type="num" val="0.3"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L35">
     <cfRule type="iconSet" priority="8">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3316,7 +3400,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3 H5:H35">
+  <conditionalFormatting sqref="F4">
     <cfRule type="iconSet" priority="7">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3327,7 +3411,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3 J5:J35">
+  <conditionalFormatting sqref="H4">
     <cfRule type="iconSet" priority="6">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3338,8 +3422,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L35">
-    <cfRule type="iconSet" priority="4">
+  <conditionalFormatting sqref="J4">
+    <cfRule type="iconSet" priority="5">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="-0.3"/>
@@ -3349,40 +3433,45 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
-    <cfRule type="iconSet" priority="3">
-      <iconSet iconSet="5Arrows">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="-0.3"/>
-        <cfvo type="num" val="-1E-3"/>
-        <cfvo type="num" val="1E-3"/>
-        <cfvo type="num" val="0.3"/>
-      </iconSet>
+  <conditionalFormatting sqref="K3:K35">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A2881F9C-3B2E-4CEC-B5F0-F6CAC0942780}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
+    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="iconSet" priority="2">
-      <iconSet iconSet="5Arrows">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="-0.3"/>
-        <cfvo type="num" val="-1E-3"/>
-        <cfvo type="num" val="1E-3"/>
-        <cfvo type="num" val="0.3"/>
-      </iconSet>
-    </cfRule>
+  <conditionalFormatting sqref="G3:G35">
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="iconSet" priority="1">
-      <iconSet iconSet="5Arrows">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="-0.3"/>
-        <cfvo type="num" val="-1E-3"/>
-        <cfvo type="num" val="1E-3"/>
-        <cfvo type="num" val="0.3"/>
-      </iconSet>
-    </cfRule>
+  <conditionalFormatting sqref="I3:I35">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A2881F9C-3B2E-4CEC-B5F0-F6CAC0942780}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K3:K35</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating table formats etc
</commit_message>
<xml_diff>
--- a/charts_and_tables/tables/formatted_xls_tables/tbl_2021_summ_incis_by_type.xlsx
+++ b/charts_and_tables/tables/formatted_xls_tables/tbl_2021_summ_incis_by_type.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy.kingham\Work\Analytical Projects\Projects\Statement_redesign\2022_annual_report_2021_report\ar-enforcement-chapter\charts_and_tables\tables\formatted_xls_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy.kingham\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -199,7 +199,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +330,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -958,151 +973,190 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1457,1932 +1511,2122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R35"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.453125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="29.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" style="4" customWidth="1"/>
-    <col min="7" max="9" width="8.7265625" style="4"/>
-    <col min="10" max="10" width="8.7265625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" style="4"/>
-    <col min="12" max="12" width="11.7265625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="9.54296875" style="4" customWidth="1"/>
-    <col min="14" max="15" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" style="4" customWidth="1"/>
-    <col min="18" max="18" width="10.7265625" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="17.1796875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="52.26953125" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.36328125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="5.36328125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.453125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="5.08984375" style="24" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="24" customWidth="1"/>
+    <col min="10" max="10" width="6.6328125" style="24" customWidth="1"/>
+    <col min="11" max="11" width="10.26953125" style="24" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" style="24" customWidth="1"/>
+    <col min="13" max="13" width="5.54296875" style="24" customWidth="1"/>
+    <col min="14" max="14" width="10.26953125" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="24" customWidth="1"/>
+    <col min="16" max="16" width="8" style="24" customWidth="1"/>
+    <col min="17" max="17" width="10.26953125" style="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.81640625" style="24" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" style="24" customWidth="1"/>
+    <col min="20" max="20" width="11.36328125" style="24" customWidth="1"/>
+    <col min="21" max="21" width="11.1796875" style="24" customWidth="1"/>
+    <col min="22" max="23" width="15.6328125" style="24" customWidth="1"/>
+    <col min="24" max="16384" width="8.7265625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:23" s="8" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="40" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="40" t="s">
+      <c r="M1" s="6"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="46" t="s">
+      <c r="P1" s="6"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="48"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="7"/>
     </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="43"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="30" t="s">
+    <row r="2" spans="1:23" s="16" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="F2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="I2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="L2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="M2" s="6"/>
+      <c r="N2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="O2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="P2" s="7"/>
+      <c r="Q2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="R2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="S2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="T2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="U2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="32" t="s">
+      <c r="V2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="W2" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="19">
         <v>31</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="41"/>
+      <c r="E3" s="20">
         <v>0.20512820512820501</v>
       </c>
-      <c r="E3" s="17">
+      <c r="F3" s="19">
         <v>78</v>
       </c>
-      <c r="F3" s="18">
+      <c r="G3" s="41"/>
+      <c r="H3" s="20">
         <v>-2.6315789473684199E-2</v>
       </c>
-      <c r="G3" s="19">
+      <c r="I3" s="21">
         <v>7.5875486381323007E-2</v>
       </c>
-      <c r="H3" s="18">
+      <c r="J3" s="44"/>
+      <c r="K3" s="20">
         <v>4.8561335244726701E-2</v>
       </c>
-      <c r="I3" s="22">
+      <c r="L3" s="22">
         <v>2.1845068055788901</v>
       </c>
-      <c r="J3" s="18">
+      <c r="M3" s="47"/>
+      <c r="N3" s="20">
         <v>-0.172016644703677</v>
       </c>
-      <c r="K3" s="25">
+      <c r="O3" s="23">
         <v>0.51428571428571401</v>
       </c>
-      <c r="L3" s="18">
+      <c r="P3" s="50"/>
+      <c r="Q3" s="20">
         <v>3.4101382488479298E-2</v>
       </c>
-      <c r="M3" s="34">
+      <c r="R3" s="53">
         <v>2.5161290322580601</v>
       </c>
-      <c r="N3" s="35">
-        <v>1</v>
-      </c>
-      <c r="O3" s="35">
-        <v>1</v>
-      </c>
-      <c r="P3" s="35">
+      <c r="S3" s="54">
+        <v>1</v>
+      </c>
+      <c r="T3" s="54">
+        <v>1</v>
+      </c>
+      <c r="U3" s="54">
         <v>20</v>
       </c>
-      <c r="Q3" s="35">
-        <v>1</v>
-      </c>
-      <c r="R3" s="36">
+      <c r="V3" s="54">
+        <v>1</v>
+      </c>
+      <c r="W3" s="55">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38"/>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="27">
         <v>0</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="42"/>
+      <c r="E4" s="28">
         <v>-1</v>
       </c>
-      <c r="E4" s="13">
+      <c r="F4" s="27">
         <v>0</v>
       </c>
-      <c r="F4" s="14">
+      <c r="G4" s="42"/>
+      <c r="H4" s="28">
         <v>-1</v>
       </c>
-      <c r="G4" s="20">
+      <c r="I4" s="31">
         <v>0</v>
       </c>
-      <c r="H4" s="14">
+      <c r="J4" s="45"/>
+      <c r="K4" s="28">
         <v>-1</v>
       </c>
-      <c r="I4" s="13">
+      <c r="L4" s="27">
         <v>0</v>
       </c>
-      <c r="J4" s="14">
+      <c r="M4" s="42"/>
+      <c r="N4" s="28">
         <v>-1</v>
       </c>
-      <c r="K4" s="26">
+      <c r="O4" s="30">
         <v>0</v>
       </c>
-      <c r="L4" s="14">
+      <c r="P4" s="51"/>
+      <c r="Q4" s="28">
         <v>-0.09</v>
       </c>
-      <c r="M4" s="5">
+      <c r="R4" s="56">
         <v>0</v>
       </c>
-      <c r="N4" s="6">
+      <c r="S4" s="57">
         <v>0</v>
       </c>
-      <c r="O4" s="6">
+      <c r="T4" s="57">
         <v>0</v>
       </c>
-      <c r="P4" s="6">
+      <c r="U4" s="57">
         <v>0</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="V4" s="57">
         <v>0</v>
       </c>
-      <c r="R4" s="7">
+      <c r="W4" s="58">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38"/>
-      <c r="B5" s="11" t="s">
+    <row r="5" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="27">
         <v>18</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="42"/>
+      <c r="E5" s="28">
         <v>-0.5</v>
       </c>
-      <c r="E5" s="13">
+      <c r="F5" s="27">
         <v>55</v>
       </c>
-      <c r="F5" s="14">
+      <c r="G5" s="42"/>
+      <c r="H5" s="28">
         <v>-1.5</v>
       </c>
-      <c r="G5" s="20">
+      <c r="I5" s="29">
         <v>5.3501945525291798E-2</v>
       </c>
-      <c r="H5" s="14">
+      <c r="J5" s="45"/>
+      <c r="K5" s="28">
         <v>-1.3176070038910499</v>
       </c>
-      <c r="I5" s="23">
+      <c r="L5" s="32">
         <v>1.5403573629081899</v>
       </c>
-      <c r="J5" s="14">
+      <c r="M5" s="48"/>
+      <c r="N5" s="28">
         <v>-1.8549123396628</v>
       </c>
-      <c r="K5" s="26">
+      <c r="O5" s="30">
         <v>0.28571428571428598</v>
       </c>
-      <c r="L5" s="14">
+      <c r="P5" s="51"/>
+      <c r="Q5" s="28">
         <v>4.6082949308756099E-3</v>
       </c>
-      <c r="M5" s="5">
+      <c r="R5" s="56">
         <v>3.0555555555555598</v>
       </c>
-      <c r="N5" s="6">
-        <v>1</v>
-      </c>
-      <c r="O5" s="6">
-        <v>1</v>
-      </c>
-      <c r="P5" s="6">
+      <c r="S5" s="57">
+        <v>1</v>
+      </c>
+      <c r="T5" s="57">
+        <v>1</v>
+      </c>
+      <c r="U5" s="57">
         <v>30</v>
       </c>
-      <c r="Q5" s="6">
-        <v>1</v>
-      </c>
-      <c r="R5" s="7">
+      <c r="V5" s="57">
+        <v>1</v>
+      </c>
+      <c r="W5" s="58">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="39"/>
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:23" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="33"/>
+      <c r="B6" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="35">
         <v>36</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="43"/>
+      <c r="E6" s="36">
         <v>0.2</v>
       </c>
-      <c r="E6" s="15">
+      <c r="F6" s="35">
         <v>87</v>
       </c>
-      <c r="F6" s="16">
+      <c r="G6" s="43"/>
+      <c r="H6" s="36">
         <v>0.51396648044692705</v>
       </c>
-      <c r="G6" s="21">
+      <c r="I6" s="37">
         <v>8.4630350194552506E-2</v>
       </c>
-      <c r="H6" s="16">
+      <c r="J6" s="46"/>
+      <c r="K6" s="36">
         <v>0.54942612438319205</v>
       </c>
-      <c r="I6" s="24">
+      <c r="L6" s="38">
         <v>2.4365652831456899</v>
       </c>
-      <c r="J6" s="16">
+      <c r="M6" s="49"/>
+      <c r="N6" s="36">
         <v>0.44496676301527699</v>
       </c>
-      <c r="K6" s="27">
+      <c r="O6" s="39">
         <v>0.6</v>
       </c>
-      <c r="L6" s="16">
+      <c r="P6" s="52"/>
+      <c r="Q6" s="36">
         <v>-5.16129032258065E-2</v>
       </c>
-      <c r="M6" s="8">
+      <c r="R6" s="59">
         <v>2.3888888888888902</v>
       </c>
-      <c r="N6" s="9">
+      <c r="S6" s="60">
         <v>2</v>
       </c>
-      <c r="O6" s="9">
+      <c r="T6" s="60">
         <v>0</v>
       </c>
-      <c r="P6" s="9">
+      <c r="U6" s="60">
         <v>10</v>
       </c>
-      <c r="Q6" s="9">
-        <v>1</v>
-      </c>
-      <c r="R6" s="10">
+      <c r="V6" s="60">
+        <v>1</v>
+      </c>
+      <c r="W6" s="61">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="19">
         <v>20</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="41"/>
+      <c r="E7" s="20">
         <v>0.28571428571428598</v>
       </c>
-      <c r="E7" s="17">
+      <c r="F7" s="19">
         <v>101</v>
       </c>
-      <c r="F7" s="18">
+      <c r="G7" s="41"/>
+      <c r="H7" s="20">
         <v>6.4814814814814797E-2</v>
       </c>
-      <c r="G7" s="19">
+      <c r="I7" s="21">
         <v>9.8249027237354097E-2</v>
       </c>
-      <c r="H7" s="18">
+      <c r="J7" s="44"/>
+      <c r="K7" s="20">
         <v>0.133043305951866</v>
       </c>
-      <c r="I7" s="22">
+      <c r="L7" s="22">
         <v>2.8286562482495898</v>
       </c>
-      <c r="J7" s="18">
+      <c r="M7" s="47"/>
+      <c r="N7" s="20">
         <v>-6.7948690022010996E-2</v>
       </c>
-      <c r="K7" s="25">
+      <c r="O7" s="23">
         <v>0.54285714285714304</v>
       </c>
-      <c r="L7" s="18">
+      <c r="P7" s="50"/>
+      <c r="Q7" s="20">
         <v>-9.1244239631336405E-2</v>
       </c>
-      <c r="M7" s="34">
+      <c r="R7" s="53">
         <v>5</v>
       </c>
-      <c r="N7" s="35">
-        <v>1</v>
-      </c>
-      <c r="O7" s="35">
+      <c r="S7" s="54">
+        <v>1</v>
+      </c>
+      <c r="T7" s="54">
         <v>0</v>
       </c>
-      <c r="P7" s="35">
+      <c r="U7" s="54">
         <v>58</v>
       </c>
-      <c r="Q7" s="35">
-        <v>1</v>
-      </c>
-      <c r="R7" s="36">
+      <c r="V7" s="54">
+        <v>1</v>
+      </c>
+      <c r="W7" s="55">
         <v>3.25</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="39"/>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:23" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="33"/>
+      <c r="B8" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="35">
         <v>63</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="43"/>
+      <c r="E8" s="36">
         <v>-0.43181818181818199</v>
       </c>
-      <c r="E8" s="15">
+      <c r="F8" s="35">
         <v>256</v>
       </c>
-      <c r="F8" s="16">
+      <c r="G8" s="43"/>
+      <c r="H8" s="36">
         <v>3.03030303030303E-2</v>
       </c>
-      <c r="G8" s="21">
+      <c r="I8" s="37">
         <v>0.249027237354086</v>
       </c>
-      <c r="H8" s="16">
+      <c r="J8" s="46"/>
+      <c r="K8" s="36">
         <v>0.10104940455135</v>
       </c>
-      <c r="I8" s="24">
+      <c r="L8" s="38">
         <v>7.1696633618999597</v>
       </c>
-      <c r="J8" s="16">
+      <c r="M8" s="49"/>
+      <c r="N8" s="36">
         <v>-0.10735993780860199</v>
       </c>
-      <c r="K8" s="27">
+      <c r="O8" s="39">
         <v>0.6</v>
       </c>
-      <c r="L8" s="16">
+      <c r="P8" s="52"/>
+      <c r="Q8" s="36">
         <v>-1.9354838709677399E-2</v>
       </c>
-      <c r="M8" s="8">
+      <c r="R8" s="59">
         <v>4.0476190476190501</v>
       </c>
-      <c r="N8" s="9">
-        <v>1</v>
-      </c>
-      <c r="O8" s="9">
+      <c r="S8" s="60">
+        <v>1</v>
+      </c>
+      <c r="T8" s="60">
         <v>0</v>
       </c>
-      <c r="P8" s="9">
+      <c r="U8" s="60">
         <v>60</v>
       </c>
-      <c r="Q8" s="9">
-        <v>1</v>
-      </c>
-      <c r="R8" s="10">
+      <c r="V8" s="60">
+        <v>1</v>
+      </c>
+      <c r="W8" s="61">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+    <row r="9" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="19">
         <v>37</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="41"/>
+      <c r="E9" s="20">
         <v>5.1282051282051301E-2</v>
       </c>
-      <c r="E9" s="17">
+      <c r="F9" s="19">
         <v>107</v>
       </c>
-      <c r="F9" s="18">
+      <c r="G9" s="41"/>
+      <c r="H9" s="20">
         <v>-0.52857142857142903</v>
       </c>
-      <c r="G9" s="19">
+      <c r="I9" s="21">
         <v>0.10408560311284</v>
       </c>
-      <c r="H9" s="18">
+      <c r="J9" s="44"/>
+      <c r="K9" s="20">
         <v>-0.41705113952195699</v>
       </c>
-      <c r="I9" s="22">
+      <c r="L9" s="22">
         <v>2.9966952332941199</v>
       </c>
-      <c r="J9" s="18">
+      <c r="M9" s="47"/>
+      <c r="N9" s="20">
         <v>-0.74557497339382806</v>
       </c>
-      <c r="K9" s="25">
+      <c r="O9" s="23">
         <v>0.57142857142857095</v>
       </c>
-      <c r="L9" s="18">
+      <c r="P9" s="50"/>
+      <c r="Q9" s="20">
         <v>-8.7557603686635899E-2</v>
       </c>
-      <c r="M9" s="34">
+      <c r="R9" s="53">
         <v>2.8918918918918899</v>
       </c>
-      <c r="N9" s="35">
-        <v>1</v>
-      </c>
-      <c r="O9" s="35">
-        <v>1</v>
-      </c>
-      <c r="P9" s="35">
+      <c r="S9" s="54">
+        <v>1</v>
+      </c>
+      <c r="T9" s="54">
+        <v>1</v>
+      </c>
+      <c r="U9" s="54">
         <v>39</v>
       </c>
-      <c r="Q9" s="35">
-        <v>1</v>
-      </c>
-      <c r="R9" s="36">
+      <c r="V9" s="54">
+        <v>1</v>
+      </c>
+      <c r="W9" s="55">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="27">
         <v>7</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="42"/>
+      <c r="E10" s="28">
         <v>-1.3333333333333299</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="27">
         <v>7</v>
       </c>
-      <c r="F10" s="14">
+      <c r="G10" s="42"/>
+      <c r="H10" s="28">
         <v>-1.3333333333333299</v>
       </c>
-      <c r="G10" s="20">
+      <c r="I10" s="29">
         <v>6.80933852140078E-3</v>
       </c>
-      <c r="H10" s="14">
+      <c r="J10" s="45"/>
+      <c r="K10" s="28">
         <v>-1.16309987029831</v>
       </c>
-      <c r="I10" s="23">
+      <c r="L10" s="32">
         <v>0.19604548255195201</v>
       </c>
-      <c r="J10" s="14">
+      <c r="M10" s="48"/>
+      <c r="N10" s="28">
         <v>-1.66458485035195</v>
       </c>
-      <c r="K10" s="26">
+      <c r="O10" s="30">
         <v>0.14285714285714299</v>
       </c>
-      <c r="L10" s="14">
+      <c r="P10" s="51"/>
+      <c r="Q10" s="28">
         <v>-4.6082949308755797E-2</v>
       </c>
-      <c r="M10" s="5">
-        <v>1</v>
-      </c>
-      <c r="N10" s="6">
-        <v>1</v>
-      </c>
-      <c r="O10" s="6">
-        <v>1</v>
-      </c>
-      <c r="P10" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>1</v>
-      </c>
-      <c r="R10" s="7">
+      <c r="R10" s="56">
+        <v>1</v>
+      </c>
+      <c r="S10" s="57">
+        <v>1</v>
+      </c>
+      <c r="T10" s="57">
+        <v>1</v>
+      </c>
+      <c r="U10" s="57">
+        <v>1</v>
+      </c>
+      <c r="V10" s="57">
+        <v>1</v>
+      </c>
+      <c r="W10" s="58">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="27">
         <v>37</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="42"/>
+      <c r="E11" s="28">
         <v>0.52564102564102599</v>
       </c>
-      <c r="E11" s="13">
+      <c r="F11" s="27">
         <v>61</v>
       </c>
-      <c r="F11" s="14">
+      <c r="G11" s="42"/>
+      <c r="H11" s="28">
         <v>0.67204301075268802</v>
       </c>
-      <c r="G11" s="20">
+      <c r="I11" s="29">
         <v>5.9338521400778201E-2</v>
       </c>
-      <c r="H11" s="14">
+      <c r="J11" s="45"/>
+      <c r="K11" s="28">
         <v>0.69596983389816303</v>
       </c>
-      <c r="I11" s="23">
+      <c r="L11" s="32">
         <v>1.70839634795273</v>
       </c>
-      <c r="J11" s="14">
+      <c r="M11" s="48"/>
+      <c r="N11" s="28">
         <v>0.62548461780767595</v>
       </c>
-      <c r="K11" s="26">
+      <c r="O11" s="30">
         <v>0.34285714285714303</v>
       </c>
-      <c r="L11" s="14">
+      <c r="P11" s="51"/>
+      <c r="Q11" s="28">
         <v>0.23778801843318001</v>
       </c>
-      <c r="M11" s="5">
+      <c r="R11" s="56">
         <v>1.64864864864865</v>
       </c>
-      <c r="N11" s="6">
-        <v>1</v>
-      </c>
-      <c r="O11" s="6">
-        <v>1</v>
-      </c>
-      <c r="P11" s="6">
+      <c r="S11" s="57">
+        <v>1</v>
+      </c>
+      <c r="T11" s="57">
+        <v>1</v>
+      </c>
+      <c r="U11" s="57">
         <v>5</v>
       </c>
-      <c r="Q11" s="6">
-        <v>1</v>
-      </c>
-      <c r="R11" s="7">
+      <c r="V11" s="57">
+        <v>1</v>
+      </c>
+      <c r="W11" s="58">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="39"/>
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:23" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="33"/>
+      <c r="B12" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="35">
         <v>125</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="43"/>
+      <c r="E12" s="36">
         <v>6.7164179104477598E-2</v>
       </c>
-      <c r="E12" s="15">
+      <c r="F12" s="35">
         <v>208</v>
       </c>
-      <c r="F12" s="16">
+      <c r="G12" s="43"/>
+      <c r="H12" s="36">
         <v>-9.7087378640776708E-3</v>
       </c>
-      <c r="G12" s="21">
+      <c r="I12" s="37">
         <v>0.202334630350195</v>
       </c>
-      <c r="H12" s="16">
+      <c r="J12" s="46"/>
+      <c r="K12" s="36">
         <v>6.3956782894488307E-2</v>
       </c>
-      <c r="I12" s="24">
+      <c r="L12" s="38">
         <v>5.82535148154372</v>
       </c>
-      <c r="J12" s="16">
+      <c r="M12" s="49"/>
+      <c r="N12" s="36">
         <v>-0.15305197407740301</v>
       </c>
-      <c r="K12" s="27">
+      <c r="O12" s="39">
         <v>0.68571428571428605</v>
       </c>
-      <c r="L12" s="16">
+      <c r="P12" s="52"/>
+      <c r="Q12" s="36">
         <v>0.12073732718893999</v>
       </c>
-      <c r="M12" s="8">
+      <c r="R12" s="59">
         <v>1.6639999999999999</v>
       </c>
-      <c r="N12" s="9">
-        <v>1</v>
-      </c>
-      <c r="O12" s="9">
-        <v>1</v>
-      </c>
-      <c r="P12" s="9">
+      <c r="S12" s="60">
+        <v>1</v>
+      </c>
+      <c r="T12" s="60">
+        <v>1</v>
+      </c>
+      <c r="U12" s="60">
         <v>6</v>
       </c>
-      <c r="Q12" s="9">
-        <v>1</v>
-      </c>
-      <c r="R12" s="10">
+      <c r="V12" s="60">
+        <v>1</v>
+      </c>
+      <c r="W12" s="61">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="37" t="s">
+    <row r="13" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="19">
         <v>23</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="41"/>
+      <c r="E13" s="20">
         <v>-0.53333333333333299</v>
       </c>
-      <c r="E13" s="17">
+      <c r="F13" s="19">
         <v>50</v>
       </c>
-      <c r="F13" s="18">
+      <c r="G13" s="41"/>
+      <c r="H13" s="20">
         <v>0.34210526315789502</v>
       </c>
-      <c r="G13" s="19">
+      <c r="I13" s="21">
         <v>4.8638132295719803E-2</v>
       </c>
-      <c r="H13" s="18">
+      <c r="J13" s="44"/>
+      <c r="K13" s="20">
         <v>0.39010342002867099</v>
       </c>
-      <c r="I13" s="22">
+      <c r="L13" s="22">
         <v>1.40032487537109</v>
       </c>
-      <c r="J13" s="18">
+      <c r="M13" s="47"/>
+      <c r="N13" s="20">
         <v>0.24870727903610501</v>
       </c>
-      <c r="K13" s="25">
+      <c r="O13" s="23">
         <v>0.25714285714285701</v>
       </c>
-      <c r="L13" s="18">
+      <c r="P13" s="50"/>
+      <c r="Q13" s="20">
         <v>-0.12811059907834099</v>
       </c>
-      <c r="M13" s="34">
+      <c r="R13" s="53">
         <v>2.1739130434782599</v>
       </c>
-      <c r="N13" s="35">
-        <v>1</v>
-      </c>
-      <c r="O13" s="35">
-        <v>1</v>
-      </c>
-      <c r="P13" s="35">
+      <c r="S13" s="54">
+        <v>1</v>
+      </c>
+      <c r="T13" s="54">
+        <v>1</v>
+      </c>
+      <c r="U13" s="54">
         <v>10</v>
       </c>
-      <c r="Q13" s="35">
-        <v>1</v>
-      </c>
-      <c r="R13" s="36">
+      <c r="V13" s="54">
+        <v>1</v>
+      </c>
+      <c r="W13" s="55">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="27">
         <v>53</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="42"/>
+      <c r="E14" s="28">
         <v>-0.15217391304347799</v>
       </c>
-      <c r="E14" s="13">
+      <c r="F14" s="27">
         <v>219</v>
       </c>
-      <c r="F14" s="14">
+      <c r="G14" s="42"/>
+      <c r="H14" s="28">
         <v>-1.8604651162790701E-2</v>
       </c>
-      <c r="G14" s="20">
+      <c r="I14" s="29">
         <v>0.21303501945525299</v>
       </c>
-      <c r="H14" s="14">
+      <c r="J14" s="45"/>
+      <c r="K14" s="28">
         <v>5.5709890507646298E-2</v>
       </c>
-      <c r="I14" s="23">
+      <c r="L14" s="32">
         <v>6.1334229541253604</v>
       </c>
-      <c r="J14" s="14">
+      <c r="M14" s="48"/>
+      <c r="N14" s="28">
         <v>-0.16321079513702999</v>
       </c>
-      <c r="K14" s="26">
+      <c r="O14" s="30">
         <v>0.2</v>
       </c>
-      <c r="L14" s="14">
+      <c r="P14" s="51"/>
+      <c r="Q14" s="28">
         <v>-6.4516129032258203E-3</v>
       </c>
-      <c r="M14" s="5">
+      <c r="R14" s="56">
         <v>4.1320754716981103</v>
       </c>
-      <c r="N14" s="6">
-        <v>1</v>
-      </c>
-      <c r="O14" s="6">
-        <v>1</v>
-      </c>
-      <c r="P14" s="6">
+      <c r="S14" s="57">
+        <v>1</v>
+      </c>
+      <c r="T14" s="57">
+        <v>1</v>
+      </c>
+      <c r="U14" s="57">
         <v>60</v>
       </c>
-      <c r="Q14" s="6">
-        <v>1</v>
-      </c>
-      <c r="R14" s="7">
+      <c r="V14" s="57">
+        <v>1</v>
+      </c>
+      <c r="W14" s="58">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="38"/>
-      <c r="B15" s="11" t="s">
+    <row r="15" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="27">
         <v>2</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="42"/>
+      <c r="E15" s="28">
         <v>0.81818181818181801</v>
       </c>
-      <c r="E15" s="13">
+      <c r="F15" s="27">
         <v>25</v>
       </c>
-      <c r="F15" s="14">
+      <c r="G15" s="42"/>
+      <c r="H15" s="28">
         <v>0.73958333333333304</v>
       </c>
-      <c r="G15" s="20">
+      <c r="I15" s="29">
         <v>2.4319066147859902E-2</v>
       </c>
-      <c r="H15" s="14">
+      <c r="J15" s="45"/>
+      <c r="K15" s="28">
         <v>0.75858260376134901</v>
       </c>
-      <c r="I15" s="23">
+      <c r="L15" s="32">
         <v>0.70016243768554298</v>
       </c>
-      <c r="J15" s="14">
+      <c r="M15" s="48"/>
+      <c r="N15" s="28">
         <v>0.70261329795179195</v>
       </c>
-      <c r="K15" s="26">
+      <c r="O15" s="30">
         <v>5.7142857142857099E-2</v>
       </c>
-      <c r="L15" s="14">
+      <c r="P15" s="51"/>
+      <c r="Q15" s="28">
         <v>7.3732718894009199E-3</v>
       </c>
-      <c r="M15" s="5">
+      <c r="R15" s="56">
         <v>12.5</v>
       </c>
-      <c r="N15" s="6">
+      <c r="S15" s="57">
         <v>12.5</v>
       </c>
-      <c r="O15" s="6">
+      <c r="T15" s="57">
         <v>2</v>
       </c>
-      <c r="P15" s="6">
+      <c r="U15" s="57">
         <v>23</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="V15" s="57">
         <v>7.25</v>
       </c>
-      <c r="R15" s="7">
+      <c r="W15" s="58">
         <v>17.75</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
-      <c r="B16" s="11" t="s">
+    <row r="16" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="27">
         <v>24</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="42"/>
+      <c r="E16" s="28">
         <v>-2.4285714285714302</v>
       </c>
-      <c r="E16" s="13">
+      <c r="F16" s="27">
         <v>160</v>
       </c>
-      <c r="F16" s="14">
+      <c r="G16" s="42"/>
+      <c r="H16" s="28">
         <v>-1.6229508196721301</v>
       </c>
-      <c r="G16" s="20">
+      <c r="I16" s="29">
         <v>0.155642023346304</v>
       </c>
-      <c r="H16" s="14">
+      <c r="J16" s="45"/>
+      <c r="K16" s="28">
         <v>-1.43158767621356</v>
       </c>
-      <c r="I16" s="23">
+      <c r="L16" s="32">
         <v>4.4810396011874802</v>
       </c>
-      <c r="J16" s="14">
+      <c r="M16" s="48"/>
+      <c r="N16" s="28">
         <v>-1.99531786456425</v>
       </c>
-      <c r="K16" s="26">
+      <c r="O16" s="30">
         <v>0.14285714285714299</v>
       </c>
-      <c r="L16" s="14">
+      <c r="P16" s="51"/>
+      <c r="Q16" s="28">
         <v>5.0691244239631297E-2</v>
       </c>
-      <c r="M16" s="5">
+      <c r="R16" s="56">
         <v>6.6666666666666696</v>
       </c>
-      <c r="N16" s="6">
-        <v>1</v>
-      </c>
-      <c r="O16" s="6">
-        <v>1</v>
-      </c>
-      <c r="P16" s="6">
+      <c r="S16" s="57">
+        <v>1</v>
+      </c>
+      <c r="T16" s="57">
+        <v>1</v>
+      </c>
+      <c r="U16" s="57">
         <v>48</v>
       </c>
-      <c r="Q16" s="6">
-        <v>1</v>
-      </c>
-      <c r="R16" s="7">
+      <c r="V16" s="57">
+        <v>1</v>
+      </c>
+      <c r="W16" s="58">
         <v>5.25</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="39"/>
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="1:23" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="33"/>
+      <c r="B17" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="15">
-        <v>1</v>
-      </c>
-      <c r="D17" s="16">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15">
-        <v>1</v>
-      </c>
-      <c r="F17" s="16">
-        <v>1</v>
-      </c>
-      <c r="G17" s="21">
+      <c r="C17" s="35">
+        <v>1</v>
+      </c>
+      <c r="D17" s="43"/>
+      <c r="E17" s="36">
+        <v>1</v>
+      </c>
+      <c r="F17" s="35">
+        <v>1</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="36">
+        <v>1</v>
+      </c>
+      <c r="I17" s="37">
         <v>9.7276264591439701E-4</v>
       </c>
-      <c r="H17" s="16">
-        <v>1</v>
-      </c>
-      <c r="I17" s="24">
+      <c r="J17" s="46"/>
+      <c r="K17" s="36">
+        <v>1</v>
+      </c>
+      <c r="L17" s="38">
         <v>2.80064975074217E-2</v>
       </c>
-      <c r="J17" s="16">
-        <v>1</v>
-      </c>
-      <c r="K17" s="27">
+      <c r="M17" s="49"/>
+      <c r="N17" s="36">
+        <v>1</v>
+      </c>
+      <c r="O17" s="39">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="L17" s="16">
+      <c r="P17" s="52"/>
+      <c r="Q17" s="36">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="M17" s="8">
-        <v>1</v>
-      </c>
-      <c r="N17" s="9">
-        <v>1</v>
-      </c>
-      <c r="O17" s="9">
-        <v>1</v>
-      </c>
-      <c r="P17" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="9">
-        <v>1</v>
-      </c>
-      <c r="R17" s="10">
+      <c r="R17" s="59">
+        <v>1</v>
+      </c>
+      <c r="S17" s="60">
+        <v>1</v>
+      </c>
+      <c r="T17" s="60">
+        <v>1</v>
+      </c>
+      <c r="U17" s="60">
+        <v>1</v>
+      </c>
+      <c r="V17" s="60">
+        <v>1</v>
+      </c>
+      <c r="W17" s="61">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="37" t="s">
+    <row r="18" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="19">
         <v>34</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="41"/>
+      <c r="E18" s="20">
         <v>0.29166666666666702</v>
       </c>
-      <c r="E18" s="17">
+      <c r="F18" s="19">
         <v>191</v>
       </c>
-      <c r="F18" s="18">
+      <c r="G18" s="41"/>
+      <c r="H18" s="20">
         <v>-0.38405797101449302</v>
       </c>
-      <c r="G18" s="19">
+      <c r="I18" s="21">
         <v>0.18579766536965001</v>
       </c>
-      <c r="H18" s="18">
+      <c r="J18" s="44"/>
+      <c r="K18" s="20">
         <v>-0.28308097896577</v>
       </c>
-      <c r="I18" s="22">
+      <c r="L18" s="22">
         <v>5.3492410239175499</v>
       </c>
-      <c r="J18" s="18">
+      <c r="M18" s="47"/>
+      <c r="N18" s="20">
         <v>-0.58054567210317398</v>
       </c>
-      <c r="K18" s="25">
+      <c r="O18" s="23">
         <v>0.2</v>
       </c>
-      <c r="L18" s="18">
+      <c r="P18" s="50"/>
+      <c r="Q18" s="20">
         <v>-6.4516129032258203E-3</v>
       </c>
-      <c r="M18" s="34">
+      <c r="R18" s="53">
         <v>5.6176470588235299</v>
       </c>
-      <c r="N18" s="35">
+      <c r="S18" s="54">
         <v>2</v>
       </c>
-      <c r="O18" s="35">
-        <v>1</v>
-      </c>
-      <c r="P18" s="35">
+      <c r="T18" s="54">
+        <v>1</v>
+      </c>
+      <c r="U18" s="54">
         <v>100</v>
       </c>
-      <c r="Q18" s="35">
-        <v>1</v>
-      </c>
-      <c r="R18" s="36">
+      <c r="V18" s="54">
+        <v>1</v>
+      </c>
+      <c r="W18" s="55">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="38"/>
-      <c r="B19" s="11" t="s">
+    <row r="19" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="25"/>
+      <c r="B19" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="27">
         <v>22</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="42"/>
+      <c r="E19" s="28">
         <v>-4.7619047619047603E-2</v>
       </c>
-      <c r="E19" s="13">
+      <c r="F19" s="27">
         <v>137</v>
       </c>
-      <c r="F19" s="14">
+      <c r="G19" s="42"/>
+      <c r="H19" s="28">
         <v>0.179640718562874</v>
       </c>
-      <c r="G19" s="20">
+      <c r="I19" s="29">
         <v>0.13326848249027201</v>
       </c>
-      <c r="H19" s="14">
+      <c r="J19" s="45"/>
+      <c r="K19" s="28">
         <v>0.239491833453715</v>
       </c>
-      <c r="I19" s="23">
+      <c r="L19" s="32">
         <v>3.8368901585167801</v>
       </c>
-      <c r="J19" s="14">
+      <c r="M19" s="48"/>
+      <c r="N19" s="28">
         <v>6.3178465787296301E-2</v>
       </c>
-      <c r="K19" s="26">
+      <c r="O19" s="30">
         <v>0.14285714285714299</v>
       </c>
-      <c r="L19" s="14">
+      <c r="P19" s="51"/>
+      <c r="Q19" s="28">
         <v>1.8433179723502301E-2</v>
       </c>
-      <c r="M19" s="5">
+      <c r="R19" s="56">
         <v>6.2272727272727302</v>
       </c>
-      <c r="N19" s="6">
-        <v>1</v>
-      </c>
-      <c r="O19" s="6">
-        <v>1</v>
-      </c>
-      <c r="P19" s="6">
+      <c r="S19" s="57">
+        <v>1</v>
+      </c>
+      <c r="T19" s="57">
+        <v>1</v>
+      </c>
+      <c r="U19" s="57">
         <v>50</v>
       </c>
-      <c r="Q19" s="6">
-        <v>1</v>
-      </c>
-      <c r="R19" s="7">
+      <c r="V19" s="57">
+        <v>1</v>
+      </c>
+      <c r="W19" s="58">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="38"/>
-      <c r="B20" s="11" t="s">
+    <row r="20" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="27">
         <v>15</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="42"/>
+      <c r="E20" s="28">
         <v>0.16666666666666699</v>
       </c>
-      <c r="E20" s="13">
+      <c r="F20" s="27">
         <v>58</v>
       </c>
-      <c r="F20" s="14">
+      <c r="G20" s="42"/>
+      <c r="H20" s="28">
         <v>-0.28888888888888897</v>
       </c>
-      <c r="G20" s="20">
+      <c r="I20" s="29">
         <v>5.6420233463034999E-2</v>
       </c>
-      <c r="H20" s="14">
+      <c r="J20" s="45"/>
+      <c r="K20" s="28">
         <v>-0.194855166450497</v>
       </c>
-      <c r="I20" s="23">
+      <c r="L20" s="32">
         <v>1.6243768554304601</v>
       </c>
-      <c r="J20" s="14">
+      <c r="M20" s="48"/>
+      <c r="N20" s="28">
         <v>-0.47186591733726702</v>
       </c>
-      <c r="K20" s="26">
+      <c r="O20" s="30">
         <v>0.14285714285714299</v>
       </c>
-      <c r="L20" s="14">
+      <c r="P20" s="51"/>
+      <c r="Q20" s="28">
         <v>5.0691244239631297E-2</v>
       </c>
-      <c r="M20" s="5">
+      <c r="R20" s="56">
         <v>3.8666666666666698</v>
       </c>
-      <c r="N20" s="6">
+      <c r="S20" s="57">
         <v>2</v>
       </c>
-      <c r="O20" s="6">
-        <v>1</v>
-      </c>
-      <c r="P20" s="6">
+      <c r="T20" s="57">
+        <v>1</v>
+      </c>
+      <c r="U20" s="57">
         <v>15</v>
       </c>
-      <c r="Q20" s="6">
-        <v>1</v>
-      </c>
-      <c r="R20" s="7">
+      <c r="V20" s="57">
+        <v>1</v>
+      </c>
+      <c r="W20" s="58">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38"/>
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="25"/>
+      <c r="B21" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="27">
         <v>20</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="42"/>
+      <c r="E21" s="28">
         <v>-5.2631578947368397E-2</v>
       </c>
-      <c r="E21" s="13">
+      <c r="F21" s="27">
         <v>691</v>
       </c>
-      <c r="F21" s="14">
+      <c r="G21" s="42"/>
+      <c r="H21" s="28">
         <v>-1.4416961130742001</v>
       </c>
-      <c r="G21" s="20">
+      <c r="I21" s="29">
         <v>0.67217898832684797</v>
       </c>
-      <c r="H21" s="14">
+      <c r="J21" s="45"/>
+      <c r="K21" s="28">
         <v>-1.26355680521373</v>
       </c>
-      <c r="I21" s="23">
+      <c r="L21" s="32">
         <v>19.352489777628399</v>
       </c>
-      <c r="J21" s="14">
+      <c r="M21" s="48"/>
+      <c r="N21" s="28">
         <v>-1.7883313451689</v>
       </c>
-      <c r="K21" s="26">
+      <c r="O21" s="30">
         <v>0.25714285714285701</v>
       </c>
-      <c r="L21" s="14">
+      <c r="P21" s="51"/>
+      <c r="Q21" s="28">
         <v>-3.1336405529953898E-2</v>
       </c>
-      <c r="M21" s="5">
+      <c r="R21" s="56">
         <v>34.549999999999997</v>
       </c>
-      <c r="N21" s="6">
+      <c r="S21" s="57">
         <v>18</v>
       </c>
-      <c r="O21" s="6">
-        <v>1</v>
-      </c>
-      <c r="P21" s="6">
+      <c r="T21" s="57">
+        <v>1</v>
+      </c>
+      <c r="U21" s="57">
         <v>400</v>
       </c>
-      <c r="Q21" s="6">
-        <v>1</v>
-      </c>
-      <c r="R21" s="7">
+      <c r="V21" s="57">
+        <v>1</v>
+      </c>
+      <c r="W21" s="58">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="38"/>
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="27">
         <v>3</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="42"/>
+      <c r="E22" s="28">
         <v>-0.5</v>
       </c>
-      <c r="E22" s="13">
+      <c r="F22" s="27">
         <v>5</v>
       </c>
-      <c r="F22" s="14">
+      <c r="G22" s="42"/>
+      <c r="H22" s="28">
         <v>-0.66666666666666696</v>
       </c>
-      <c r="G22" s="20">
+      <c r="I22" s="29">
         <v>4.8638132295719802E-3</v>
       </c>
-      <c r="H22" s="14">
+      <c r="J22" s="45"/>
+      <c r="K22" s="28">
         <v>-0.54507133592736701</v>
       </c>
-      <c r="I22" s="23">
+      <c r="L22" s="32">
         <v>0.14003248753710901</v>
       </c>
-      <c r="J22" s="14">
+      <c r="M22" s="48"/>
+      <c r="N22" s="28">
         <v>-0.90327489310853504</v>
       </c>
-      <c r="K22" s="26">
+      <c r="O22" s="30">
         <v>0.17142857142857101</v>
       </c>
-      <c r="L22" s="14">
+      <c r="P22" s="51"/>
+      <c r="Q22" s="28">
         <v>-0.10691244239631301</v>
       </c>
-      <c r="M22" s="5">
+      <c r="R22" s="56">
         <v>1.6666666666666701</v>
       </c>
-      <c r="N22" s="6">
+      <c r="S22" s="57">
         <v>2</v>
       </c>
-      <c r="O22" s="6">
-        <v>1</v>
-      </c>
-      <c r="P22" s="6">
+      <c r="T22" s="57">
+        <v>1</v>
+      </c>
+      <c r="U22" s="57">
         <v>2</v>
       </c>
-      <c r="Q22" s="6">
+      <c r="V22" s="57">
         <v>1.5</v>
       </c>
-      <c r="R22" s="7">
+      <c r="W22" s="58">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="38"/>
-      <c r="B23" s="11" t="s">
+    <row r="23" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="27">
         <v>27</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="42"/>
+      <c r="E23" s="28">
         <v>0.27027027027027001</v>
       </c>
-      <c r="E23" s="13">
+      <c r="F23" s="27">
         <v>147</v>
       </c>
-      <c r="F23" s="14">
+      <c r="G23" s="42"/>
+      <c r="H23" s="28">
         <v>1.34228187919463E-2</v>
       </c>
-      <c r="G23" s="20">
+      <c r="I23" s="29">
         <v>0.142996108949416</v>
       </c>
-      <c r="H23" s="14">
+      <c r="J23" s="45"/>
+      <c r="K23" s="28">
         <v>8.5400725981249898E-2</v>
       </c>
-      <c r="I23" s="23">
+      <c r="L23" s="32">
         <v>4.1169551335909897</v>
       </c>
-      <c r="J23" s="14">
+      <c r="M23" s="48"/>
+      <c r="N23" s="28">
         <v>-0.12663654746424599</v>
       </c>
-      <c r="K23" s="26">
+      <c r="O23" s="30">
         <v>0.57142857142857095</v>
       </c>
-      <c r="L23" s="14">
+      <c r="P23" s="51"/>
+      <c r="Q23" s="28">
         <v>-5.5299539170506902E-2</v>
       </c>
-      <c r="M23" s="5">
+      <c r="R23" s="56">
         <v>5.4444444444444402</v>
       </c>
-      <c r="N23" s="6">
-        <v>1</v>
-      </c>
-      <c r="O23" s="6">
-        <v>1</v>
-      </c>
-      <c r="P23" s="6">
+      <c r="S23" s="57">
+        <v>1</v>
+      </c>
+      <c r="T23" s="57">
+        <v>1</v>
+      </c>
+      <c r="U23" s="57">
         <v>50</v>
       </c>
-      <c r="Q23" s="6">
-        <v>1</v>
-      </c>
-      <c r="R23" s="7">
+      <c r="V23" s="57">
+        <v>1</v>
+      </c>
+      <c r="W23" s="58">
         <v>3.5</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="38"/>
-      <c r="B24" s="11" t="s">
+    <row r="24" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="25"/>
+      <c r="B24" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="27">
         <v>3</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="42"/>
+      <c r="E24" s="28">
         <v>0.4</v>
       </c>
-      <c r="E24" s="13">
+      <c r="F24" s="27">
         <v>14</v>
       </c>
-      <c r="F24" s="14">
+      <c r="G24" s="42"/>
+      <c r="H24" s="28">
         <v>0.875</v>
       </c>
-      <c r="G24" s="20">
+      <c r="I24" s="29">
         <v>1.36186770428016E-2</v>
       </c>
-      <c r="H24" s="14">
+      <c r="J24" s="45"/>
+      <c r="K24" s="28">
         <v>0.88411964980544699</v>
       </c>
-      <c r="I24" s="23">
+      <c r="L24" s="32">
         <v>0.39209096510390401</v>
       </c>
-      <c r="J24" s="14">
+      <c r="M24" s="48"/>
+      <c r="N24" s="28">
         <v>0.85725438301685997</v>
       </c>
-      <c r="K24" s="26">
+      <c r="O24" s="30">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="L24" s="14">
+      <c r="P24" s="51"/>
+      <c r="Q24" s="28">
         <v>1.10599078341014E-2</v>
       </c>
-      <c r="M24" s="5">
+      <c r="R24" s="56">
         <v>4.6666666666666696</v>
       </c>
-      <c r="N24" s="6">
-        <v>1</v>
-      </c>
-      <c r="O24" s="6">
-        <v>1</v>
-      </c>
-      <c r="P24" s="6">
+      <c r="S24" s="57">
+        <v>1</v>
+      </c>
+      <c r="T24" s="57">
+        <v>1</v>
+      </c>
+      <c r="U24" s="57">
         <v>12</v>
       </c>
-      <c r="Q24" s="6">
-        <v>1</v>
-      </c>
-      <c r="R24" s="7">
+      <c r="V24" s="57">
+        <v>1</v>
+      </c>
+      <c r="W24" s="58">
         <v>6.5</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="38"/>
-      <c r="B25" s="11" t="s">
+    <row r="25" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="25"/>
+      <c r="B25" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="13">
-        <v>1</v>
-      </c>
-      <c r="D25" s="14">
-        <v>1</v>
-      </c>
-      <c r="E25" s="13">
-        <v>1</v>
-      </c>
-      <c r="F25" s="14">
-        <v>1</v>
-      </c>
-      <c r="G25" s="20">
+      <c r="C25" s="27">
+        <v>1</v>
+      </c>
+      <c r="D25" s="42"/>
+      <c r="E25" s="28">
+        <v>1</v>
+      </c>
+      <c r="F25" s="27">
+        <v>1</v>
+      </c>
+      <c r="G25" s="42"/>
+      <c r="H25" s="28">
+        <v>1</v>
+      </c>
+      <c r="I25" s="29">
         <v>9.7276264591439701E-4</v>
       </c>
-      <c r="H25" s="14">
-        <v>1</v>
-      </c>
-      <c r="I25" s="23">
+      <c r="J25" s="45"/>
+      <c r="K25" s="28">
+        <v>1</v>
+      </c>
+      <c r="L25" s="32">
         <v>2.80064975074217E-2</v>
       </c>
-      <c r="J25" s="14">
-        <v>1</v>
-      </c>
-      <c r="K25" s="26">
+      <c r="M25" s="48"/>
+      <c r="N25" s="28">
+        <v>1</v>
+      </c>
+      <c r="O25" s="30">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="L25" s="14">
+      <c r="P25" s="51"/>
+      <c r="Q25" s="28">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="M25" s="5">
-        <v>1</v>
-      </c>
-      <c r="N25" s="6">
-        <v>1</v>
-      </c>
-      <c r="O25" s="6">
-        <v>1</v>
-      </c>
-      <c r="P25" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="6">
-        <v>1</v>
-      </c>
-      <c r="R25" s="7">
+      <c r="R25" s="56">
+        <v>1</v>
+      </c>
+      <c r="S25" s="57">
+        <v>1</v>
+      </c>
+      <c r="T25" s="57">
+        <v>1</v>
+      </c>
+      <c r="U25" s="57">
+        <v>1</v>
+      </c>
+      <c r="V25" s="57">
+        <v>1</v>
+      </c>
+      <c r="W25" s="58">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="38"/>
-      <c r="B26" s="11" t="s">
+    <row r="26" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="25"/>
+      <c r="B26" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="27">
         <v>2</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="42"/>
+      <c r="E26" s="28">
         <v>-1</v>
       </c>
-      <c r="E26" s="13">
+      <c r="F26" s="27">
         <v>30</v>
       </c>
-      <c r="F26" s="14">
+      <c r="G26" s="42"/>
+      <c r="H26" s="28">
         <v>-1</v>
       </c>
-      <c r="G26" s="20">
+      <c r="I26" s="29">
         <v>2.91828793774319E-2</v>
       </c>
-      <c r="H26" s="14">
+      <c r="J26" s="45"/>
+      <c r="K26" s="28">
         <v>-0.85408560311284099</v>
       </c>
-      <c r="I26" s="23">
+      <c r="L26" s="32">
         <v>0.84019492522265204</v>
       </c>
-      <c r="J26" s="14">
+      <c r="M26" s="48"/>
+      <c r="N26" s="28">
         <v>-1.2839298717302401</v>
       </c>
-      <c r="K26" s="26">
+      <c r="O26" s="30">
         <v>5.7142857142857099E-2</v>
       </c>
-      <c r="L26" s="14">
+      <c r="P26" s="51"/>
+      <c r="Q26" s="28">
         <v>-2.4884792626728099E-2</v>
       </c>
-      <c r="M26" s="5">
+      <c r="R26" s="56">
         <v>15</v>
       </c>
-      <c r="N26" s="6">
+      <c r="S26" s="57">
         <v>15</v>
       </c>
-      <c r="O26" s="6">
+      <c r="T26" s="57">
         <v>10</v>
       </c>
-      <c r="P26" s="6">
+      <c r="U26" s="57">
         <v>20</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="V26" s="57">
         <v>12.5</v>
       </c>
-      <c r="R26" s="7">
+      <c r="W26" s="58">
         <v>17.5</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="39"/>
-      <c r="B27" s="12" t="s">
+    <row r="27" spans="1:23" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="33"/>
+      <c r="B27" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="35">
         <v>3</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="43"/>
+      <c r="E27" s="36">
         <v>-0.5</v>
       </c>
-      <c r="E27" s="15">
+      <c r="F27" s="35">
         <v>4</v>
       </c>
-      <c r="F27" s="16">
+      <c r="G27" s="43"/>
+      <c r="H27" s="36">
         <v>-0.33333333333333298</v>
       </c>
-      <c r="G27" s="21">
+      <c r="I27" s="37">
         <v>3.8910505836575902E-3</v>
       </c>
-      <c r="H27" s="16">
+      <c r="J27" s="46"/>
+      <c r="K27" s="36">
         <v>-0.236057068741894</v>
       </c>
-      <c r="I27" s="24">
+      <c r="L27" s="38">
         <v>0.11202599002968699</v>
       </c>
-      <c r="J27" s="16">
+      <c r="M27" s="49"/>
+      <c r="N27" s="36">
         <v>-0.52261991448682799</v>
       </c>
-      <c r="K27" s="27">
+      <c r="O27" s="39">
         <v>8.5714285714285701E-2</v>
       </c>
-      <c r="L27" s="16">
+      <c r="P27" s="52"/>
+      <c r="Q27" s="36">
         <v>-5.3456221198156698E-2</v>
       </c>
-      <c r="M27" s="8">
+      <c r="R27" s="59">
         <v>1.3333333333333299</v>
       </c>
-      <c r="N27" s="9">
-        <v>1</v>
-      </c>
-      <c r="O27" s="9">
-        <v>1</v>
-      </c>
-      <c r="P27" s="9">
+      <c r="S27" s="60">
+        <v>1</v>
+      </c>
+      <c r="T27" s="60">
+        <v>1</v>
+      </c>
+      <c r="U27" s="60">
         <v>2</v>
       </c>
-      <c r="Q27" s="9">
-        <v>1</v>
-      </c>
-      <c r="R27" s="10">
+      <c r="V27" s="60">
+        <v>1</v>
+      </c>
+      <c r="W27" s="61">
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="38" t="s">
+    <row r="28" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="13">
+      <c r="B28" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="27">
         <v>25</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="42"/>
+      <c r="E28" s="28">
         <v>-0.78571428571428603</v>
       </c>
-      <c r="E28" s="13">
+      <c r="F28" s="27">
         <v>38</v>
       </c>
-      <c r="F28" s="14">
+      <c r="G28" s="42"/>
+      <c r="H28" s="28">
         <v>-0.52</v>
       </c>
-      <c r="G28" s="20">
+      <c r="I28" s="29">
         <v>3.6964980544747103E-2</v>
       </c>
-      <c r="H28" s="14">
+      <c r="J28" s="45"/>
+      <c r="K28" s="28">
         <v>-0.409105058365759</v>
       </c>
-      <c r="I28" s="23">
+      <c r="L28" s="32">
         <v>1.06424690528203</v>
       </c>
-      <c r="J28" s="14">
+      <c r="M28" s="48"/>
+      <c r="N28" s="28">
         <v>-0.73578670251498302</v>
       </c>
-      <c r="K28" s="26">
+      <c r="O28" s="30">
         <v>0.45714285714285702</v>
       </c>
-      <c r="L28" s="14">
+      <c r="P28" s="51"/>
+      <c r="Q28" s="28">
         <v>-0.13456221198156701</v>
       </c>
-      <c r="M28" s="5">
+      <c r="R28" s="56">
         <v>1.52</v>
       </c>
-      <c r="N28" s="6">
-        <v>1</v>
-      </c>
-      <c r="O28" s="6">
-        <v>1</v>
-      </c>
-      <c r="P28" s="6">
+      <c r="S28" s="57">
+        <v>1</v>
+      </c>
+      <c r="T28" s="57">
+        <v>1</v>
+      </c>
+      <c r="U28" s="57">
         <v>4</v>
       </c>
-      <c r="Q28" s="6">
-        <v>1</v>
-      </c>
-      <c r="R28" s="7">
+      <c r="V28" s="57">
+        <v>1</v>
+      </c>
+      <c r="W28" s="58">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="38"/>
-      <c r="B29" s="11" t="s">
+    <row r="29" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="25"/>
+      <c r="B29" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="27">
         <v>26</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="42"/>
+      <c r="E29" s="28">
         <v>0.31578947368421101</v>
       </c>
-      <c r="E29" s="13">
+      <c r="F29" s="27">
         <v>309</v>
       </c>
-      <c r="F29" s="14">
+      <c r="G29" s="42"/>
+      <c r="H29" s="28">
         <v>-0.21176470588235299</v>
       </c>
-      <c r="G29" s="20">
+      <c r="I29" s="29">
         <v>0.30058365758754901</v>
       </c>
-      <c r="H29" s="14">
+      <c r="J29" s="45"/>
+      <c r="K29" s="28">
         <v>-0.123357747768368</v>
       </c>
-      <c r="I29" s="23">
+      <c r="L29" s="32">
         <v>8.6540077297933102</v>
       </c>
-      <c r="J29" s="14">
+      <c r="M29" s="48"/>
+      <c r="N29" s="28">
         <v>-0.38379280463655802</v>
       </c>
-      <c r="K29" s="26">
+      <c r="O29" s="30">
         <v>0.28571428571428598</v>
       </c>
-      <c r="L29" s="14">
+      <c r="P29" s="51"/>
+      <c r="Q29" s="28">
         <v>0.29493087557603698</v>
       </c>
-      <c r="M29" s="5">
+      <c r="R29" s="56">
         <v>11.884615384615399</v>
       </c>
-      <c r="N29" s="6">
+      <c r="S29" s="57">
         <v>2</v>
       </c>
-      <c r="O29" s="6">
-        <v>1</v>
-      </c>
-      <c r="P29" s="6">
+      <c r="T29" s="57">
+        <v>1</v>
+      </c>
+      <c r="U29" s="57">
         <v>100</v>
       </c>
-      <c r="Q29" s="6">
-        <v>1</v>
-      </c>
-      <c r="R29" s="7">
+      <c r="V29" s="57">
+        <v>1</v>
+      </c>
+      <c r="W29" s="58">
         <v>7.5</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="38"/>
-      <c r="B30" s="11" t="s">
+    <row r="30" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="25"/>
+      <c r="B30" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="27">
         <v>18</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="42"/>
+      <c r="E30" s="28">
         <v>-5.8823529411764698E-2</v>
       </c>
-      <c r="E30" s="13">
+      <c r="F30" s="27">
         <v>71</v>
       </c>
-      <c r="F30" s="14">
+      <c r="G30" s="42"/>
+      <c r="H30" s="28">
         <v>-0.22413793103448301</v>
       </c>
-      <c r="G30" s="20">
+      <c r="I30" s="29">
         <v>6.9066147859922197E-2</v>
       </c>
-      <c r="H30" s="14">
+      <c r="J30" s="45"/>
+      <c r="K30" s="28">
         <v>-0.134828257077687</v>
       </c>
-      <c r="I30" s="23">
+      <c r="L30" s="32">
         <v>1.9884613230269399</v>
       </c>
-      <c r="J30" s="14">
+      <c r="M30" s="48"/>
+      <c r="N30" s="28">
         <v>-0.39792259390385498</v>
       </c>
-      <c r="K30" s="26">
+      <c r="O30" s="30">
         <v>0.314285714285714</v>
       </c>
-      <c r="L30" s="14">
+      <c r="P30" s="51"/>
+      <c r="Q30" s="28">
         <v>-5.6221198156682001E-2</v>
       </c>
-      <c r="M30" s="5">
+      <c r="R30" s="56">
         <v>3.9444444444444402</v>
       </c>
-      <c r="N30" s="6">
-        <v>1</v>
-      </c>
-      <c r="O30" s="6">
-        <v>1</v>
-      </c>
-      <c r="P30" s="6">
+      <c r="S30" s="57">
+        <v>1</v>
+      </c>
+      <c r="T30" s="57">
+        <v>1</v>
+      </c>
+      <c r="U30" s="57">
         <v>40</v>
       </c>
-      <c r="Q30" s="6">
-        <v>1</v>
-      </c>
-      <c r="R30" s="7">
+      <c r="V30" s="57">
+        <v>1</v>
+      </c>
+      <c r="W30" s="58">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="38"/>
-      <c r="B31" s="11" t="s">
+    <row r="31" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="25"/>
+      <c r="B31" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="27">
         <v>8</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="42"/>
+      <c r="E31" s="28">
         <v>-0.6</v>
       </c>
-      <c r="E31" s="13">
+      <c r="F31" s="27">
         <v>66</v>
       </c>
-      <c r="F31" s="14">
+      <c r="G31" s="42"/>
+      <c r="H31" s="28">
         <v>-2.8823529411764701</v>
       </c>
-      <c r="G31" s="20">
+      <c r="I31" s="29">
         <v>6.4202334630350202E-2</v>
       </c>
-      <c r="H31" s="14">
+      <c r="J31" s="45"/>
+      <c r="K31" s="28">
         <v>-2.5991073472190398</v>
       </c>
-      <c r="I31" s="23">
+      <c r="L31" s="32">
         <v>1.8484288354898299</v>
       </c>
-      <c r="J31" s="14">
+      <c r="M31" s="48"/>
+      <c r="N31" s="28">
         <v>-3.43351092747635</v>
       </c>
-      <c r="K31" s="26">
+      <c r="O31" s="30">
         <v>0.17142857142857101</v>
       </c>
-      <c r="L31" s="14">
+      <c r="P31" s="51"/>
+      <c r="Q31" s="28">
         <v>8.6635944700460807E-2</v>
       </c>
-      <c r="M31" s="5">
+      <c r="R31" s="56">
         <v>8.25</v>
       </c>
-      <c r="N31" s="6">
+      <c r="S31" s="57">
         <v>7</v>
       </c>
-      <c r="O31" s="6">
-        <v>1</v>
-      </c>
-      <c r="P31" s="6">
+      <c r="T31" s="57">
+        <v>1</v>
+      </c>
+      <c r="U31" s="57">
         <v>23</v>
       </c>
-      <c r="Q31" s="6">
+      <c r="V31" s="57">
         <v>1.75</v>
       </c>
-      <c r="R31" s="7">
+      <c r="W31" s="58">
         <v>11.25</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="38"/>
-      <c r="B32" s="11" t="s">
+    <row r="32" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="25"/>
+      <c r="B32" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="27">
         <v>12</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="42"/>
+      <c r="E32" s="28">
         <v>-0.33333333333333298</v>
       </c>
-      <c r="E32" s="13">
+      <c r="F32" s="27">
         <v>30</v>
       </c>
-      <c r="F32" s="14">
+      <c r="G32" s="42"/>
+      <c r="H32" s="28">
         <v>-2.3333333333333299</v>
       </c>
-      <c r="G32" s="20">
+      <c r="I32" s="29">
         <v>2.91828793774319E-2</v>
       </c>
-      <c r="H32" s="14">
+      <c r="J32" s="45"/>
+      <c r="K32" s="28">
         <v>-2.0901426718547298</v>
       </c>
-      <c r="I32" s="23">
+      <c r="L32" s="32">
         <v>0.84019492522265204</v>
       </c>
-      <c r="J32" s="14">
+      <c r="M32" s="48"/>
+      <c r="N32" s="28">
         <v>-2.8065497862170701</v>
       </c>
-      <c r="K32" s="26">
+      <c r="O32" s="30">
         <v>0.25714285714285701</v>
       </c>
-      <c r="L32" s="14">
+      <c r="P32" s="51"/>
+      <c r="Q32" s="28">
         <v>3.3179723502304199E-2</v>
       </c>
-      <c r="M32" s="5">
+      <c r="R32" s="56">
         <v>2.5</v>
       </c>
-      <c r="N32" s="6">
-        <v>1</v>
-      </c>
-      <c r="O32" s="6">
-        <v>1</v>
-      </c>
-      <c r="P32" s="6">
+      <c r="S32" s="57">
+        <v>1</v>
+      </c>
+      <c r="T32" s="57">
+        <v>1</v>
+      </c>
+      <c r="U32" s="57">
         <v>10</v>
       </c>
-      <c r="Q32" s="6">
-        <v>1</v>
-      </c>
-      <c r="R32" s="7">
+      <c r="V32" s="57">
+        <v>1</v>
+      </c>
+      <c r="W32" s="58">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="38"/>
-      <c r="B33" s="11" t="s">
+    <row r="33" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="25"/>
+      <c r="B33" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="27">
         <v>25</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="42"/>
+      <c r="E33" s="28">
         <v>7.4074074074074098E-2</v>
       </c>
-      <c r="E33" s="13">
+      <c r="F33" s="27">
         <v>184</v>
       </c>
-      <c r="F33" s="14">
+      <c r="G33" s="42"/>
+      <c r="H33" s="28">
         <v>-5.7471264367816098E-2</v>
       </c>
-      <c r="G33" s="20">
+      <c r="I33" s="29">
         <v>0.178988326848249</v>
       </c>
-      <c r="H33" s="14">
+      <c r="J33" s="45"/>
+      <c r="K33" s="28">
         <v>1.9678876515049799E-2</v>
       </c>
-      <c r="I33" s="23">
+      <c r="L33" s="32">
         <v>5.1531955413655997</v>
       </c>
-      <c r="J33" s="14">
+      <c r="M33" s="48"/>
+      <c r="N33" s="28">
         <v>-0.20759510459300101</v>
       </c>
-      <c r="K33" s="26">
+      <c r="O33" s="30">
         <v>0.51428571428571401</v>
       </c>
-      <c r="L33" s="14">
+      <c r="P33" s="51"/>
+      <c r="Q33" s="28">
         <v>3.4101382488479298E-2</v>
       </c>
-      <c r="M33" s="5">
+      <c r="R33" s="56">
         <v>7.36</v>
       </c>
-      <c r="N33" s="6">
-        <v>1</v>
-      </c>
-      <c r="O33" s="6">
-        <v>1</v>
-      </c>
-      <c r="P33" s="6">
+      <c r="S33" s="57">
+        <v>1</v>
+      </c>
+      <c r="T33" s="57">
+        <v>1</v>
+      </c>
+      <c r="U33" s="57">
         <v>70</v>
       </c>
-      <c r="Q33" s="6">
-        <v>1</v>
-      </c>
-      <c r="R33" s="7">
+      <c r="V33" s="57">
+        <v>1</v>
+      </c>
+      <c r="W33" s="58">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="38"/>
-      <c r="B34" s="11" t="s">
+    <row r="34" spans="1:23" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="25"/>
+      <c r="B34" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="27">
         <v>89</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="42"/>
+      <c r="E34" s="28">
         <v>2.1978021978022001E-2</v>
       </c>
-      <c r="E34" s="13">
+      <c r="F34" s="27">
         <v>792</v>
       </c>
-      <c r="F34" s="14">
+      <c r="G34" s="42"/>
+      <c r="H34" s="28">
         <v>-2.9908972691807499E-2</v>
       </c>
-      <c r="G34" s="20">
+      <c r="I34" s="29">
         <v>0.77042801556420204</v>
       </c>
-      <c r="H34" s="14">
+      <c r="J34" s="45"/>
+      <c r="K34" s="28">
         <v>4.5230300607692002E-2</v>
       </c>
-      <c r="I34" s="23">
+      <c r="L34" s="32">
         <v>22.181146025878</v>
       </c>
-      <c r="J34" s="14">
+      <c r="M34" s="48"/>
+      <c r="N34" s="28">
         <v>-0.176119933946912</v>
       </c>
-      <c r="K34" s="26">
+      <c r="O34" s="30">
         <v>0.82857142857142896</v>
       </c>
-      <c r="L34" s="14">
+      <c r="P34" s="51"/>
+      <c r="Q34" s="28">
         <v>-2.21198156682029E-2</v>
       </c>
-      <c r="M34" s="5">
+      <c r="R34" s="56">
         <v>8.8988764044943807</v>
       </c>
-      <c r="N34" s="6">
+      <c r="S34" s="57">
         <v>2</v>
       </c>
-      <c r="O34" s="6">
-        <v>1</v>
-      </c>
-      <c r="P34" s="6">
+      <c r="T34" s="57">
+        <v>1</v>
+      </c>
+      <c r="U34" s="57">
         <v>102</v>
       </c>
-      <c r="Q34" s="6">
-        <v>1</v>
-      </c>
-      <c r="R34" s="7">
+      <c r="V34" s="57">
+        <v>1</v>
+      </c>
+      <c r="W34" s="58">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="39.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="39"/>
-      <c r="B35" s="12" t="s">
+    <row r="35" spans="1:23" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="33"/>
+      <c r="B35" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="15">
+      <c r="C35" s="35">
         <v>8</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="43"/>
+      <c r="E35" s="36">
         <v>-0.14285714285714299</v>
       </c>
-      <c r="E35" s="15">
+      <c r="F35" s="35">
         <v>71</v>
       </c>
-      <c r="F35" s="16">
+      <c r="G35" s="43"/>
+      <c r="H35" s="36">
         <v>0.15476190476190499</v>
       </c>
-      <c r="G35" s="21">
+      <c r="I35" s="37">
         <v>6.9066147859922197E-2</v>
       </c>
-      <c r="H35" s="16">
+      <c r="J35" s="46"/>
+      <c r="K35" s="36">
         <v>0.216428108208264</v>
       </c>
-      <c r="I35" s="24">
+      <c r="L35" s="38">
         <v>1.9884613230269399</v>
       </c>
-      <c r="J35" s="16">
+      <c r="M35" s="49"/>
+      <c r="N35" s="36">
         <v>3.4767732780671898E-2</v>
       </c>
-      <c r="K35" s="27">
+      <c r="O35" s="39">
         <v>0.34285714285714303</v>
       </c>
-      <c r="L35" s="16">
+      <c r="P35" s="52"/>
+      <c r="Q35" s="36">
         <v>-0.14930875576036901</v>
       </c>
-      <c r="M35" s="8">
+      <c r="R35" s="59">
         <v>8.875</v>
       </c>
-      <c r="N35" s="9">
+      <c r="S35" s="60">
         <v>4</v>
       </c>
-      <c r="O35" s="9">
-        <v>1</v>
-      </c>
-      <c r="P35" s="9">
+      <c r="T35" s="60">
+        <v>1</v>
+      </c>
+      <c r="U35" s="60">
         <v>30</v>
       </c>
-      <c r="Q35" s="9">
-        <v>1</v>
-      </c>
-      <c r="R35" s="10">
+      <c r="V35" s="60">
+        <v>1</v>
+      </c>
+      <c r="W35" s="61">
         <v>12.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="A13:A17"/>
+  <mergeCells count="19">
     <mergeCell ref="A18:A27"/>
     <mergeCell ref="A28:A35"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="C1:E1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A12"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:D35">
+  <conditionalFormatting sqref="E3:E35">
     <cfRule type="iconSet" priority="13">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3393,7 +3637,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3 F5:F35">
+  <conditionalFormatting sqref="H3 H5:H35">
     <cfRule type="iconSet" priority="12">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3404,7 +3648,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3 H5:H35">
+  <conditionalFormatting sqref="K3 K5:K35">
     <cfRule type="iconSet" priority="11">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3415,7 +3659,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3 J5:J35">
+  <conditionalFormatting sqref="N3 N5:N35">
     <cfRule type="iconSet" priority="10">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3426,7 +3670,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L35">
+  <conditionalFormatting sqref="Q3:Q35">
     <cfRule type="iconSet" priority="8">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3437,7 +3681,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="H4">
     <cfRule type="iconSet" priority="7">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3448,7 +3692,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
+  <conditionalFormatting sqref="K4">
     <cfRule type="iconSet" priority="6">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3459,7 +3703,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
+  <conditionalFormatting sqref="N4">
     <cfRule type="iconSet" priority="5">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
@@ -3470,7 +3714,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K35">
+  <conditionalFormatting sqref="O3:P35">
+    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -3483,16 +3728,15 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G35">
+  <conditionalFormatting sqref="I3:J35">
     <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I35">
+  <conditionalFormatting sqref="L3:M35">
     <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="44" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -3505,7 +3749,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K3:K35</xm:sqref>
+          <xm:sqref>O3:P35</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>